<commit_message>
Created pie chart for 2015 sales data
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\madtroll\Documents\GitHub\ECON431ResearchPaper\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joseph\OneDrive\UofL\2016_Spring\ECON 431\Research_Paper\ECON431ResearchPaper\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9195"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
   </bookViews>
   <sheets>
     <sheet name="DISTILLED SPIRITS - VALUE" sheetId="1" r:id="rId1"/>
@@ -455,7 +455,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -522,14 +522,11 @@
   </cellStyleXfs>
   <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -540,9 +537,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -561,6 +561,1349 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1440" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1440" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>DISTILLED SPIRITS - EXPORTS BY VALUE (U.S. DOLLARS)</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1440" b="0" i="0" u="none" strike="noStrike" baseline="0"/>
+              <a:t> - </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>2015</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1440" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:ofPieChart>
+        <c:ofPieType val="pie"/>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'DISTILLED SPIRITS - VALUE'!$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2015</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-C4AE-4C49-8BA3-064E80B79DED}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000006-C4AE-4C49-8BA3-064E80B79DED}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-C4AE-4C49-8BA3-064E80B79DED}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000008-C4AE-4C49-8BA3-064E80B79DED}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000004-C4AE-4C49-8BA3-064E80B79DED}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="8"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-C4AE-4C49-8BA3-064E80B79DED}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="9"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-C4AE-4C49-8BA3-064E80B79DED}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.139745170571311"/>
+                  <c:y val="-7.3387408265739681E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-C4AE-4C49-8BA3-064E80B79DED}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-2.055076037813399E-3"/>
+                  <c:y val="5.7937427578215531E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000006-C4AE-4C49-8BA3-064E80B79DED}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="4.3156596794081362E-2"/>
+                  <c:y val="7.3387408265739668E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000007-C4AE-4C49-8BA3-064E80B79DED}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0"/>
+                  <c:y val="9.656237929702588E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000008-C4AE-4C49-8BA3-064E80B79DED}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-2.306021858241826E-2"/>
+                  <c:y val="6.1799922750096561E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{34B7A188-D640-43F5-AD43-1C9FB2AB1FCF}" type="CATEGORYNAME">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CATEGORY NAME]</a:t>
+                    </a:fld>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t>
+&lt;1%</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-C4AE-4C49-8BA3-064E80B79DED}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="8"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-3.904644471845458E-2"/>
+                  <c:y val="-8.8837388953263804E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>Tequila &lt;1%</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-C4AE-4C49-8BA3-064E80B79DED}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="9"/>
+              <c:layout/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>Whiskey</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t>
+</a:t>
+                    </a:r>
+                    <a:fld id="{688B430C-C531-4E81-B75F-270ED27F49D4}" type="PERCENTAGE">
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:pPr/>
+                      <a:t>[PERCENTAGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US" baseline="0"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-C4AE-4C49-8BA3-064E80B79DED}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="35000"/>
+                      <a:lumOff val="65000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'DISTILLED SPIRITS - VALUE'!$A$3:$A$12</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>('DISTILLED SPIRITS - VALUE'!$A$3:$A$4,'DISTILLED SPIRITS - VALUE'!$A$6:$A$12)</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>WHISKEY, BOURBON</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>WHISKEY, OTHER</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>RUM</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>BRANDY</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>GIN</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>VODKA</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>CORDIALS</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>OTHER DISTILLED SPIRITS</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>TEQUILA</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'DISTILLED SPIRITS - VALUE'!$B$3:$B$12</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>('DISTILLED SPIRITS - VALUE'!$B$3:$B$4,'DISTILLED SPIRITS - VALUE'!$B$6:$B$12)</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>722755084</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>355497190</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>93158899</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>93782350</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6884192</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>63622174</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>90663881</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>138492124</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5621518</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+              <c15:categoryFilterExceptions/>
+            </c:ext>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C4AE-4C49-8BA3-064E80B79DED}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:gapWidth val="100"/>
+        <c:splitType val="cust"/>
+        <c:custSplit>
+          <c:secondPiePt val="0"/>
+          <c:secondPiePt val="1"/>
+          <c:secondPiePt val="9"/>
+        </c:custSplit>
+        <c:secondPieSize val="74"/>
+        <c:serLines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="35000"/>
+                  <a:lumOff val="65000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:serLines>
+      </c:ofPieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="333">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1440" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>15240</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>601980</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -639,23 +1982,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -691,23 +2017,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -863,42 +2172,42 @@
   <dimension ref="A1:H144"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="14.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="9">
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B2" s="8">
         <v>2015</v>
       </c>
-      <c r="C2" s="10">
+      <c r="C2" s="9">
         <v>2014</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -917,7 +2226,7 @@
         <v>-0.29278945678074986</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -936,28 +2245,28 @@
         <v>3.9220748397218541</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="4">
         <f>SUM(B2:B4)</f>
         <v>1078254289</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="4">
         <f>SUM(C2:C4)</f>
         <v>1094207157</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="5">
         <f t="shared" si="0"/>
         <v>-15952868</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="6">
         <f t="shared" si="1"/>
         <v>-1.4579385537687541E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -976,7 +2285,7 @@
         <v>-4.4109246429455476E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -995,7 +2304,7 @@
         <v>0.10578721487089715</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -1014,7 +2323,7 @@
         <v>0.40280144922220457</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -1033,7 +2342,7 @@
         <v>0.2474933876972453</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -1052,7 +2361,7 @@
         <v>1.4043532638193336E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -1071,7 +2380,7 @@
         <v>-9.7530641305369845E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -1090,49 +2399,49 @@
         <v>-0.15490434281413923</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B13" s="4">
         <f>SUM(B6:B12)</f>
         <v>492225138</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="4">
         <f>SUM(C6:C12)</f>
         <v>474091992</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D13" s="5">
         <f t="shared" si="0"/>
         <v>18133146</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E13" s="6">
         <f t="shared" si="1"/>
         <v>3.8248159230666774E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B14" s="4">
         <f>SUM(B13,B5)</f>
         <v>1570479427</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="4">
         <f>SUM(C13,C5)</f>
         <v>1568299149</v>
       </c>
-      <c r="D14" s="6">
+      <c r="D14" s="5">
         <f t="shared" si="0"/>
         <v>2180278</v>
       </c>
-      <c r="E14" s="7">
+      <c r="E14" s="6">
         <f t="shared" si="1"/>
         <v>1.3902181872573343E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B19">
         <v>2015</v>
       </c>
@@ -1152,7 +2461,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>15</v>
       </c>
@@ -1162,11 +2471,11 @@
       <c r="C20" s="1">
         <v>153007</v>
       </c>
-      <c r="D20" s="11">
+      <c r="D20" s="10">
         <f t="shared" ref="D20" si="2">B20-C20</f>
         <v>-153007</v>
       </c>
-      <c r="E20" s="12">
+      <c r="E20" s="11">
         <f>IF(C20=0,"NEW",D20/C20)</f>
         <v>-1</v>
       </c>
@@ -1179,7 +2488,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>16</v>
       </c>
@@ -1189,16 +2498,16 @@
       <c r="C21" s="1">
         <v>115461</v>
       </c>
-      <c r="D21" s="11">
+      <c r="D21" s="10">
         <f t="shared" ref="D21:D84" si="3">B21-C21</f>
         <v>-115461</v>
       </c>
-      <c r="E21" s="12">
+      <c r="E21" s="11">
         <f t="shared" ref="E21:E84" si="4">IF(C21=0,"NEW",D21/C21)</f>
         <v>-1</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>17</v>
       </c>
@@ -1208,16 +2517,16 @@
       <c r="C22" s="1">
         <v>47349</v>
       </c>
-      <c r="D22" s="11">
+      <c r="D22" s="10">
         <f t="shared" si="3"/>
         <v>5490</v>
       </c>
-      <c r="E22" s="12">
+      <c r="E22" s="11">
         <f t="shared" si="4"/>
         <v>0.11594753849078122</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>18</v>
       </c>
@@ -1227,16 +2536,16 @@
       <c r="C23" s="1">
         <v>1076602</v>
       </c>
-      <c r="D23" s="11">
+      <c r="D23" s="10">
         <f t="shared" si="3"/>
         <v>-343355</v>
       </c>
-      <c r="E23" s="12">
+      <c r="E23" s="11">
         <f t="shared" si="4"/>
         <v>-0.31892472798675836</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>19</v>
       </c>
@@ -1246,16 +2555,16 @@
       <c r="C24" s="1">
         <v>41640</v>
       </c>
-      <c r="D24" s="11">
+      <c r="D24" s="10">
         <f t="shared" si="3"/>
         <v>-41640</v>
       </c>
-      <c r="E24" s="12">
+      <c r="E24" s="11">
         <f t="shared" si="4"/>
         <v>-1</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>20</v>
       </c>
@@ -1265,16 +2574,16 @@
       <c r="C25" s="1">
         <v>102812427</v>
       </c>
-      <c r="D25" s="11">
+      <c r="D25" s="10">
         <f t="shared" si="3"/>
         <v>-32387261</v>
       </c>
-      <c r="E25" s="12">
+      <c r="E25" s="11">
         <f t="shared" si="4"/>
         <v>-0.31501309661720173</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>21</v>
       </c>
@@ -1284,16 +2593,16 @@
       <c r="C26" s="1">
         <v>7795106</v>
       </c>
-      <c r="D26" s="11">
+      <c r="D26" s="10">
         <f t="shared" si="3"/>
         <v>-4181579</v>
       </c>
-      <c r="E26" s="12">
+      <c r="E26" s="11">
         <f t="shared" si="4"/>
         <v>-0.53643645128109863</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>22</v>
       </c>
@@ -1303,16 +2612,16 @@
       <c r="C27" s="1">
         <v>527689</v>
       </c>
-      <c r="D27" s="11">
+      <c r="D27" s="10">
         <f t="shared" si="3"/>
         <v>-105587</v>
       </c>
-      <c r="E27" s="12">
+      <c r="E27" s="11">
         <f t="shared" si="4"/>
         <v>-0.20009323673603202</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>23</v>
       </c>
@@ -1322,16 +2631,16 @@
       <c r="C28" s="1">
         <v>380204</v>
       </c>
-      <c r="D28" s="11">
+      <c r="D28" s="10">
         <f t="shared" si="3"/>
         <v>-46156</v>
       </c>
-      <c r="E28" s="12">
+      <c r="E28" s="11">
         <f t="shared" si="4"/>
         <v>-0.12139798634417313</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>24</v>
       </c>
@@ -1341,16 +2650,16 @@
       <c r="C29" s="1">
         <v>0</v>
       </c>
-      <c r="D29" s="11">
+      <c r="D29" s="10">
         <f t="shared" si="3"/>
         <v>65469</v>
       </c>
-      <c r="E29" s="12" t="str">
+      <c r="E29" s="11" t="str">
         <f t="shared" si="4"/>
         <v>NEW</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>25</v>
       </c>
@@ -1360,16 +2669,16 @@
       <c r="C30" s="1">
         <v>0</v>
       </c>
-      <c r="D30" s="11">
+      <c r="D30" s="10">
         <f t="shared" si="3"/>
         <v>36527</v>
       </c>
-      <c r="E30" s="12" t="str">
+      <c r="E30" s="11" t="str">
         <f t="shared" si="4"/>
         <v>NEW</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>26</v>
       </c>
@@ -1379,16 +2688,16 @@
       <c r="C31" s="1">
         <v>76354</v>
       </c>
-      <c r="D31" s="11">
+      <c r="D31" s="10">
         <f t="shared" si="3"/>
         <v>5484</v>
       </c>
-      <c r="E31" s="12">
+      <c r="E31" s="11">
         <f t="shared" si="4"/>
         <v>7.1823349136914891E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>27</v>
       </c>
@@ -1398,16 +2707,16 @@
       <c r="C32" s="1">
         <v>18660355</v>
       </c>
-      <c r="D32" s="11">
+      <c r="D32" s="10">
         <f t="shared" si="3"/>
         <v>-7751612</v>
       </c>
-      <c r="E32" s="12">
+      <c r="E32" s="11">
         <f t="shared" si="4"/>
         <v>-0.41540538751808315</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>28</v>
       </c>
@@ -1417,16 +2726,16 @@
       <c r="C33" s="1">
         <v>693272</v>
       </c>
-      <c r="D33" s="11">
+      <c r="D33" s="10">
         <f t="shared" si="3"/>
         <v>-153130</v>
       </c>
-      <c r="E33" s="12">
+      <c r="E33" s="11">
         <f t="shared" si="4"/>
         <v>-0.22088011631798196</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>29</v>
       </c>
@@ -1436,16 +2745,16 @@
       <c r="C34" s="1">
         <v>5302363</v>
       </c>
-      <c r="D34" s="11">
+      <c r="D34" s="10">
         <f t="shared" si="3"/>
         <v>-3465018</v>
       </c>
-      <c r="E34" s="12">
+      <c r="E34" s="11">
         <f t="shared" si="4"/>
         <v>-0.65348562518258368</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>30</v>
       </c>
@@ -1455,16 +2764,16 @@
       <c r="C35" s="1">
         <v>17070</v>
       </c>
-      <c r="D35" s="11">
+      <c r="D35" s="10">
         <f t="shared" si="3"/>
         <v>31803</v>
       </c>
-      <c r="E35" s="12">
+      <c r="E35" s="11">
         <f t="shared" si="4"/>
         <v>1.8630931458699473</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>31</v>
       </c>
@@ -1474,16 +2783,16 @@
       <c r="C36" s="1">
         <v>143790</v>
       </c>
-      <c r="D36" s="11">
+      <c r="D36" s="10">
         <f t="shared" si="3"/>
         <v>-143790</v>
       </c>
-      <c r="E36" s="12">
+      <c r="E36" s="11">
         <f t="shared" si="4"/>
         <v>-1</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>32</v>
       </c>
@@ -1493,16 +2802,16 @@
       <c r="C37" s="1">
         <v>6987958</v>
       </c>
-      <c r="D37" s="11">
+      <c r="D37" s="10">
         <f t="shared" si="3"/>
         <v>-1529330</v>
       </c>
-      <c r="E37" s="12">
+      <c r="E37" s="11">
         <f t="shared" si="4"/>
         <v>-0.21885220260339286</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>33</v>
       </c>
@@ -1512,16 +2821,16 @@
       <c r="C38" s="1">
         <v>6402257</v>
       </c>
-      <c r="D38" s="11">
+      <c r="D38" s="10">
         <f t="shared" si="3"/>
         <v>-2506783</v>
       </c>
-      <c r="E38" s="12">
+      <c r="E38" s="11">
         <f t="shared" si="4"/>
         <v>-0.39154676233709457</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>34</v>
       </c>
@@ -1531,16 +2840,16 @@
       <c r="C39" s="1">
         <v>697485</v>
       </c>
-      <c r="D39" s="11">
+      <c r="D39" s="10">
         <f t="shared" si="3"/>
         <v>-378325</v>
       </c>
-      <c r="E39" s="12">
+      <c r="E39" s="11">
         <f t="shared" si="4"/>
         <v>-0.5424130984895732</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>35</v>
       </c>
@@ -1550,16 +2859,16 @@
       <c r="C40" s="1">
         <v>7737</v>
       </c>
-      <c r="D40" s="11">
+      <c r="D40" s="10">
         <f t="shared" si="3"/>
         <v>-7737</v>
       </c>
-      <c r="E40" s="12">
+      <c r="E40" s="11">
         <f t="shared" si="4"/>
         <v>-1</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>36</v>
       </c>
@@ -1569,16 +2878,16 @@
       <c r="C41" s="1">
         <v>33423004</v>
       </c>
-      <c r="D41" s="11">
+      <c r="D41" s="10">
         <f t="shared" si="3"/>
         <v>869067</v>
       </c>
-      <c r="E41" s="12">
+      <c r="E41" s="11">
         <f t="shared" si="4"/>
         <v>2.6002061334762131E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>37</v>
       </c>
@@ -1588,16 +2897,16 @@
       <c r="C42" s="1">
         <v>30835</v>
       </c>
-      <c r="D42" s="11">
+      <c r="D42" s="10">
         <f t="shared" si="3"/>
         <v>23582</v>
       </c>
-      <c r="E42" s="12">
+      <c r="E42" s="11">
         <f t="shared" si="4"/>
         <v>0.76478028214691096</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>38</v>
       </c>
@@ -1607,16 +2916,16 @@
       <c r="C43" s="1">
         <v>12390236</v>
       </c>
-      <c r="D43" s="11">
+      <c r="D43" s="10">
         <f t="shared" si="3"/>
         <v>-5675966</v>
       </c>
-      <c r="E43" s="12">
+      <c r="E43" s="11">
         <f t="shared" si="4"/>
         <v>-0.45809991028419472</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>39</v>
       </c>
@@ -1626,16 +2935,16 @@
       <c r="C44" s="1">
         <v>4467702</v>
       </c>
-      <c r="D44" s="11">
+      <c r="D44" s="10">
         <f t="shared" si="3"/>
         <v>-297612</v>
       </c>
-      <c r="E44" s="12">
+      <c r="E44" s="11">
         <f t="shared" si="4"/>
         <v>-6.6614111684261845E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>40</v>
       </c>
@@ -1645,16 +2954,16 @@
       <c r="C45" s="1">
         <v>988890</v>
       </c>
-      <c r="D45" s="11">
+      <c r="D45" s="10">
         <f t="shared" si="3"/>
         <v>-86681</v>
       </c>
-      <c r="E45" s="12">
+      <c r="E45" s="11">
         <f t="shared" si="4"/>
         <v>-8.7654845331634465E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>41</v>
       </c>
@@ -1664,16 +2973,16 @@
       <c r="C46" s="1">
         <v>34450</v>
       </c>
-      <c r="D46" s="11">
+      <c r="D46" s="10">
         <f t="shared" si="3"/>
         <v>-34450</v>
       </c>
-      <c r="E46" s="12">
+      <c r="E46" s="11">
         <f t="shared" si="4"/>
         <v>-1</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>42</v>
       </c>
@@ -1683,16 +2992,16 @@
       <c r="C47" s="1">
         <v>86307</v>
       </c>
-      <c r="D47" s="11">
+      <c r="D47" s="10">
         <f t="shared" si="3"/>
         <v>96339</v>
       </c>
-      <c r="E47" s="12">
+      <c r="E47" s="11">
         <f t="shared" si="4"/>
         <v>1.1162362264937955</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>43</v>
       </c>
@@ -1702,16 +3011,16 @@
       <c r="C48" s="1">
         <v>3743552</v>
       </c>
-      <c r="D48" s="11">
+      <c r="D48" s="10">
         <f t="shared" si="3"/>
         <v>-1618224</v>
       </c>
-      <c r="E48" s="12">
+      <c r="E48" s="11">
         <f t="shared" si="4"/>
         <v>-0.43226967329424032</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>44</v>
       </c>
@@ -1721,16 +3030,16 @@
       <c r="C49" s="1">
         <v>0</v>
       </c>
-      <c r="D49" s="11">
+      <c r="D49" s="10">
         <f t="shared" si="3"/>
         <v>56385</v>
       </c>
-      <c r="E49" s="12" t="str">
+      <c r="E49" s="11" t="str">
         <f t="shared" si="4"/>
         <v>NEW</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>45</v>
       </c>
@@ -1740,16 +3049,16 @@
       <c r="C50" s="1">
         <v>64583</v>
       </c>
-      <c r="D50" s="11">
+      <c r="D50" s="10">
         <f t="shared" si="3"/>
         <v>-49928</v>
       </c>
-      <c r="E50" s="12">
+      <c r="E50" s="11">
         <f t="shared" si="4"/>
         <v>-0.77308269978167632</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>46</v>
       </c>
@@ -1759,16 +3068,16 @@
       <c r="C51" s="1">
         <v>1245685</v>
       </c>
-      <c r="D51" s="11">
+      <c r="D51" s="10">
         <f t="shared" si="3"/>
         <v>-339817</v>
       </c>
-      <c r="E51" s="12">
+      <c r="E51" s="11">
         <f t="shared" si="4"/>
         <v>-0.27279528933879754</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>49</v>
       </c>
@@ -1778,16 +3087,16 @@
       <c r="C52" s="1">
         <v>3738190</v>
       </c>
-      <c r="D52" s="11">
+      <c r="D52" s="10">
         <f t="shared" si="3"/>
         <v>-2653643</v>
       </c>
-      <c r="E52" s="12">
+      <c r="E52" s="11">
         <f t="shared" si="4"/>
         <v>-0.70987376243583122</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>47</v>
       </c>
@@ -1797,16 +3106,16 @@
       <c r="C53" s="1">
         <v>2284321</v>
       </c>
-      <c r="D53" s="11">
+      <c r="D53" s="10">
         <f t="shared" si="3"/>
         <v>-498151</v>
       </c>
-      <c r="E53" s="12">
+      <c r="E53" s="11">
         <f t="shared" si="4"/>
         <v>-0.21807399222788743</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>48</v>
       </c>
@@ -1816,16 +3125,16 @@
       <c r="C54" s="1">
         <v>592724</v>
       </c>
-      <c r="D54" s="11">
+      <c r="D54" s="10">
         <f t="shared" si="3"/>
         <v>-142610</v>
       </c>
-      <c r="E54" s="12">
+      <c r="E54" s="11">
         <f t="shared" si="4"/>
         <v>-0.24060102172343284</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>50</v>
       </c>
@@ -1835,16 +3144,16 @@
       <c r="C55" s="1">
         <v>11776</v>
       </c>
-      <c r="D55" s="11">
+      <c r="D55" s="10">
         <f t="shared" si="3"/>
         <v>11197</v>
       </c>
-      <c r="E55" s="12">
+      <c r="E55" s="11">
         <f t="shared" si="4"/>
         <v>0.95083220108695654</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>51</v>
       </c>
@@ -1854,16 +3163,16 @@
       <c r="C56" s="1">
         <v>1710177</v>
       </c>
-      <c r="D56" s="11">
+      <c r="D56" s="10">
         <f t="shared" si="3"/>
         <v>-706519</v>
       </c>
-      <c r="E56" s="12">
+      <c r="E56" s="11">
         <f t="shared" si="4"/>
         <v>-0.41312624365782019</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>52</v>
       </c>
@@ -1873,16 +3182,16 @@
       <c r="C57" s="1">
         <v>2064191</v>
       </c>
-      <c r="D57" s="11">
+      <c r="D57" s="10">
         <f t="shared" si="3"/>
         <v>-1816116</v>
       </c>
-      <c r="E57" s="12">
+      <c r="E57" s="11">
         <f t="shared" si="4"/>
         <v>-0.87981974536271113</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>53</v>
       </c>
@@ -1892,16 +3201,16 @@
       <c r="C58" s="1">
         <v>6780</v>
       </c>
-      <c r="D58" s="11">
+      <c r="D58" s="10">
         <f t="shared" si="3"/>
         <v>5828</v>
       </c>
-      <c r="E58" s="12">
+      <c r="E58" s="11">
         <f t="shared" si="4"/>
         <v>0.85958702064896753</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>54</v>
       </c>
@@ -1911,16 +3220,16 @@
       <c r="C59" s="1">
         <v>2802152</v>
       </c>
-      <c r="D59" s="11">
+      <c r="D59" s="10">
         <f t="shared" si="3"/>
         <v>-757550</v>
       </c>
-      <c r="E59" s="12">
+      <c r="E59" s="11">
         <f t="shared" si="4"/>
         <v>-0.27034579137748416</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>55</v>
       </c>
@@ -1930,16 +3239,16 @@
       <c r="C60" s="1">
         <v>232960</v>
       </c>
-      <c r="D60" s="11">
+      <c r="D60" s="10">
         <f t="shared" si="3"/>
         <v>-136360</v>
       </c>
-      <c r="E60" s="12">
+      <c r="E60" s="11">
         <f t="shared" si="4"/>
         <v>-0.58533653846153844</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>56</v>
       </c>
@@ -1949,16 +3258,16 @@
       <c r="C61" s="1">
         <v>260354</v>
       </c>
-      <c r="D61" s="11">
+      <c r="D61" s="10">
         <f t="shared" si="3"/>
         <v>-157547</v>
       </c>
-      <c r="E61" s="12">
+      <c r="E61" s="11">
         <f t="shared" si="4"/>
         <v>-0.60512609754411306</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>57</v>
       </c>
@@ -1968,16 +3277,16 @@
       <c r="C62" s="1">
         <v>101571505</v>
       </c>
-      <c r="D62" s="11">
+      <c r="D62" s="10">
         <f t="shared" si="3"/>
         <v>-49489842</v>
       </c>
-      <c r="E62" s="12">
+      <c r="E62" s="11">
         <f t="shared" si="4"/>
         <v>-0.48724139708277436</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>58</v>
       </c>
@@ -1987,16 +3296,16 @@
       <c r="C63" s="1">
         <v>7788444</v>
       </c>
-      <c r="D63" s="11">
+      <c r="D63" s="10">
         <f t="shared" si="3"/>
         <v>-2726291</v>
       </c>
-      <c r="E63" s="12">
+      <c r="E63" s="11">
         <f t="shared" si="4"/>
         <v>-0.35004308947974716</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>59</v>
       </c>
@@ -2006,16 +3315,16 @@
       <c r="C64" s="1">
         <v>96610083</v>
       </c>
-      <c r="D64" s="11">
+      <c r="D64" s="10">
         <f t="shared" si="3"/>
         <v>-45760759</v>
       </c>
-      <c r="E64" s="12">
+      <c r="E64" s="11">
         <f t="shared" si="4"/>
         <v>-0.47366442072097176</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>60</v>
       </c>
@@ -2025,16 +3334,16 @@
       <c r="C65" s="1">
         <v>9798667</v>
       </c>
-      <c r="D65" s="11">
+      <c r="D65" s="10">
         <f t="shared" si="3"/>
         <v>-7414582</v>
       </c>
-      <c r="E65" s="12">
+      <c r="E65" s="11">
         <f t="shared" si="4"/>
         <v>-0.75669292568060531</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>61</v>
       </c>
@@ -2044,16 +3353,16 @@
       <c r="C66" s="1">
         <v>9251</v>
       </c>
-      <c r="D66" s="11">
+      <c r="D66" s="10">
         <f t="shared" si="3"/>
         <v>-9251</v>
       </c>
-      <c r="E66" s="12">
+      <c r="E66" s="11">
         <f t="shared" si="4"/>
         <v>-1</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>62</v>
       </c>
@@ -2063,16 +3372,16 @@
       <c r="C67" s="1">
         <v>273521</v>
       </c>
-      <c r="D67" s="11">
+      <c r="D67" s="10">
         <f t="shared" si="3"/>
         <v>-44652</v>
       </c>
-      <c r="E67" s="12">
+      <c r="E67" s="11">
         <f t="shared" si="4"/>
         <v>-0.16324889130999082</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>63</v>
       </c>
@@ -2082,16 +3391,16 @@
       <c r="C68" s="1">
         <v>277910</v>
       </c>
-      <c r="D68" s="11">
+      <c r="D68" s="10">
         <f t="shared" si="3"/>
         <v>-184618</v>
       </c>
-      <c r="E68" s="12">
+      <c r="E68" s="11">
         <f t="shared" si="4"/>
         <v>-0.66430858911158286</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>64</v>
       </c>
@@ -2101,16 +3410,16 @@
       <c r="C69" s="1">
         <v>3037</v>
       </c>
-      <c r="D69" s="11">
+      <c r="D69" s="10">
         <f t="shared" si="3"/>
         <v>-3037</v>
       </c>
-      <c r="E69" s="12">
+      <c r="E69" s="11">
         <f t="shared" si="4"/>
         <v>-1</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>65</v>
       </c>
@@ -2120,16 +3429,16 @@
       <c r="C70" s="1">
         <v>88965</v>
       </c>
-      <c r="D70" s="11">
+      <c r="D70" s="10">
         <f t="shared" si="3"/>
         <v>-33480</v>
       </c>
-      <c r="E70" s="12">
+      <c r="E70" s="11">
         <f t="shared" si="4"/>
         <v>-0.37632776934749623</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>66</v>
       </c>
@@ -2139,16 +3448,16 @@
       <c r="C71" s="1">
         <v>29625</v>
       </c>
-      <c r="D71" s="11">
+      <c r="D71" s="10">
         <f t="shared" si="3"/>
         <v>-11325</v>
       </c>
-      <c r="E71" s="12">
+      <c r="E71" s="11">
         <f t="shared" si="4"/>
         <v>-0.38227848101265821</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>67</v>
       </c>
@@ -2158,16 +3467,16 @@
       <c r="C72" s="1">
         <v>2232330</v>
       </c>
-      <c r="D72" s="11">
+      <c r="D72" s="10">
         <f t="shared" si="3"/>
         <v>-616390</v>
       </c>
-      <c r="E72" s="12">
+      <c r="E72" s="11">
         <f t="shared" si="4"/>
         <v>-0.27611957013523986</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>68</v>
       </c>
@@ -2177,16 +3486,16 @@
       <c r="C73" s="1">
         <v>2295573</v>
       </c>
-      <c r="D73" s="11">
+      <c r="D73" s="10">
         <f t="shared" si="3"/>
         <v>-1136652</v>
       </c>
-      <c r="E73" s="12">
+      <c r="E73" s="11">
         <f t="shared" si="4"/>
         <v>-0.49514957703370793</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>69</v>
       </c>
@@ -2196,16 +3505,16 @@
       <c r="C74" s="1">
         <v>222096</v>
       </c>
-      <c r="D74" s="11">
+      <c r="D74" s="10">
         <f t="shared" si="3"/>
         <v>-131686</v>
       </c>
-      <c r="E74" s="12">
+      <c r="E74" s="11">
         <f t="shared" si="4"/>
         <v>-0.59292378070744178</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>70</v>
       </c>
@@ -2215,16 +3524,16 @@
       <c r="C75" s="1">
         <v>3582648</v>
       </c>
-      <c r="D75" s="11">
+      <c r="D75" s="10">
         <f t="shared" si="3"/>
         <v>-1597432</v>
       </c>
-      <c r="E75" s="12">
+      <c r="E75" s="11">
         <f t="shared" si="4"/>
         <v>-0.44588025393507819</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>71</v>
       </c>
@@ -2234,16 +3543,16 @@
       <c r="C76" s="1">
         <v>0</v>
       </c>
-      <c r="D76" s="11">
+      <c r="D76" s="10">
         <f t="shared" si="3"/>
         <v>9098</v>
       </c>
-      <c r="E76" s="12" t="str">
+      <c r="E76" s="11" t="str">
         <f t="shared" si="4"/>
         <v>NEW</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>72</v>
       </c>
@@ -2253,16 +3562,16 @@
       <c r="C77" s="1">
         <v>4075159</v>
       </c>
-      <c r="D77" s="11">
+      <c r="D77" s="10">
         <f t="shared" si="3"/>
         <v>-1489200</v>
       </c>
-      <c r="E77" s="12">
+      <c r="E77" s="11">
         <f t="shared" si="4"/>
         <v>-0.36543359412479365</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>73</v>
       </c>
@@ -2272,16 +3581,16 @@
       <c r="C78" s="1">
         <v>3406976</v>
       </c>
-      <c r="D78" s="11">
+      <c r="D78" s="10">
         <f t="shared" si="3"/>
         <v>-830819</v>
       </c>
-      <c r="E78" s="12">
+      <c r="E78" s="11">
         <f t="shared" si="4"/>
         <v>-0.24385818978472404</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>74</v>
       </c>
@@ -2291,16 +3600,16 @@
       <c r="C79" s="1">
         <v>27439305</v>
       </c>
-      <c r="D79" s="11">
+      <c r="D79" s="10">
         <f t="shared" si="3"/>
         <v>-13090702</v>
       </c>
-      <c r="E79" s="12">
+      <c r="E79" s="11">
         <f t="shared" si="4"/>
         <v>-0.4770784828551598</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>75</v>
       </c>
@@ -2310,16 +3619,16 @@
       <c r="C80" s="1">
         <v>444958</v>
       </c>
-      <c r="D80" s="11">
+      <c r="D80" s="10">
         <f t="shared" si="3"/>
         <v>-5234</v>
       </c>
-      <c r="E80" s="12">
+      <c r="E80" s="11">
         <f t="shared" si="4"/>
         <v>-1.176290795985239E-2</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>76</v>
       </c>
@@ -2329,16 +3638,16 @@
       <c r="C81" s="1">
         <v>72882617</v>
       </c>
-      <c r="D81" s="11">
+      <c r="D81" s="10">
         <f t="shared" si="3"/>
         <v>-135720</v>
       </c>
-      <c r="E81" s="12">
+      <c r="E81" s="11">
         <f t="shared" si="4"/>
         <v>-1.862172429949929E-3</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>77</v>
       </c>
@@ -2348,16 +3657,16 @@
       <c r="C82" s="1">
         <v>261558</v>
       </c>
-      <c r="D82" s="11">
+      <c r="D82" s="10">
         <f t="shared" si="3"/>
         <v>-39992</v>
       </c>
-      <c r="E82" s="12">
+      <c r="E82" s="11">
         <f t="shared" si="4"/>
         <v>-0.15289916576820436</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>78</v>
       </c>
@@ -2367,16 +3676,16 @@
       <c r="C83" s="1">
         <v>65205</v>
       </c>
-      <c r="D83" s="11">
+      <c r="D83" s="10">
         <f t="shared" si="3"/>
         <v>-4515</v>
       </c>
-      <c r="E83" s="12">
+      <c r="E83" s="11">
         <f t="shared" si="4"/>
         <v>-6.9243156199677941E-2</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>79</v>
       </c>
@@ -2386,16 +3695,16 @@
       <c r="C84" s="1">
         <v>12046</v>
       </c>
-      <c r="D84" s="11">
+      <c r="D84" s="10">
         <f t="shared" si="3"/>
         <v>-3811</v>
       </c>
-      <c r="E84" s="12">
+      <c r="E84" s="11">
         <f t="shared" si="4"/>
         <v>-0.3163705794454591</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>80</v>
       </c>
@@ -2405,16 +3714,16 @@
       <c r="C85" s="1">
         <v>2826572</v>
       </c>
-      <c r="D85" s="11">
+      <c r="D85" s="10">
         <f t="shared" ref="D85:D144" si="5">B85-C85</f>
         <v>-492746</v>
       </c>
-      <c r="E85" s="12">
+      <c r="E85" s="11">
         <f t="shared" ref="E85:E144" si="6">IF(C85=0,"NEW",D85/C85)</f>
         <v>-0.17432635715630099</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>81</v>
       </c>
@@ -2424,16 +3733,16 @@
       <c r="C86" s="1">
         <v>23501652</v>
       </c>
-      <c r="D86" s="11">
+      <c r="D86" s="10">
         <f t="shared" si="5"/>
         <v>7463495</v>
       </c>
-      <c r="E86" s="12">
+      <c r="E86" s="11">
         <f t="shared" si="6"/>
         <v>0.31757320719411553</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>82</v>
       </c>
@@ -2443,16 +3752,16 @@
       <c r="C87" s="1">
         <v>1081764</v>
       </c>
-      <c r="D87" s="11">
+      <c r="D87" s="10">
         <f t="shared" si="5"/>
         <v>-575164</v>
       </c>
-      <c r="E87" s="12">
+      <c r="E87" s="11">
         <f t="shared" si="6"/>
         <v>-0.5316908309021191</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>83</v>
       </c>
@@ -2462,16 +3771,16 @@
       <c r="C88" s="1">
         <v>4125306</v>
       </c>
-      <c r="D88" s="11">
+      <c r="D88" s="10">
         <f t="shared" si="5"/>
         <v>-1380134</v>
       </c>
-      <c r="E88" s="12">
+      <c r="E88" s="11">
         <f t="shared" si="6"/>
         <v>-0.33455312163509809</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>84</v>
       </c>
@@ -2481,16 +3790,16 @@
       <c r="C89" s="1">
         <v>10570</v>
       </c>
-      <c r="D89" s="11">
+      <c r="D89" s="10">
         <f t="shared" si="5"/>
         <v>232080</v>
       </c>
-      <c r="E89" s="12">
+      <c r="E89" s="11">
         <f t="shared" si="6"/>
         <v>21.956480605487229</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>85</v>
       </c>
@@ -2500,16 +3809,16 @@
       <c r="C90" s="1">
         <v>19210</v>
       </c>
-      <c r="D90" s="11">
+      <c r="D90" s="10">
         <f t="shared" si="5"/>
         <v>-11410</v>
       </c>
-      <c r="E90" s="12">
+      <c r="E90" s="11">
         <f t="shared" si="6"/>
         <v>-0.59396147839666835</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>86</v>
       </c>
@@ -2519,16 +3828,16 @@
       <c r="C91" s="1">
         <v>105290</v>
       </c>
-      <c r="D91" s="11">
+      <c r="D91" s="10">
         <f t="shared" si="5"/>
         <v>-34998</v>
       </c>
-      <c r="E91" s="12">
+      <c r="E91" s="11">
         <f t="shared" si="6"/>
         <v>-0.33239623895906545</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>87</v>
       </c>
@@ -2538,16 +3847,16 @@
       <c r="C92" s="1">
         <v>1145273</v>
       </c>
-      <c r="D92" s="11">
+      <c r="D92" s="10">
         <f t="shared" si="5"/>
         <v>-547479</v>
       </c>
-      <c r="E92" s="12">
+      <c r="E92" s="11">
         <f t="shared" si="6"/>
         <v>-0.47803362167797547</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>88</v>
       </c>
@@ -2557,16 +3866,16 @@
       <c r="C93" s="1">
         <v>0</v>
       </c>
-      <c r="D93" s="11">
+      <c r="D93" s="10">
         <f t="shared" si="5"/>
         <v>23793</v>
       </c>
-      <c r="E93" s="12" t="str">
+      <c r="E93" s="11" t="str">
         <f t="shared" si="6"/>
         <v>NEW</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>89</v>
       </c>
@@ -2576,16 +3885,16 @@
       <c r="C94" s="1">
         <v>569363</v>
       </c>
-      <c r="D94" s="11">
+      <c r="D94" s="10">
         <f t="shared" si="5"/>
         <v>-343069</v>
       </c>
-      <c r="E94" s="12">
+      <c r="E94" s="11">
         <f t="shared" si="6"/>
         <v>-0.60254881332295918</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>90</v>
       </c>
@@ -2595,16 +3904,16 @@
       <c r="C95" s="1">
         <v>10043085</v>
       </c>
-      <c r="D95" s="11">
+      <c r="D95" s="10">
         <f t="shared" si="5"/>
         <v>-1358279</v>
       </c>
-      <c r="E95" s="12">
+      <c r="E95" s="11">
         <f t="shared" si="6"/>
         <v>-0.13524519607272067</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>91</v>
       </c>
@@ -2614,16 +3923,16 @@
       <c r="C96" s="1">
         <v>350114</v>
       </c>
-      <c r="D96" s="11">
+      <c r="D96" s="10">
         <f t="shared" si="5"/>
         <v>-78978</v>
       </c>
-      <c r="E96" s="12">
+      <c r="E96" s="11">
         <f t="shared" si="6"/>
         <v>-0.22557795460907018</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>92</v>
       </c>
@@ -2633,16 +3942,16 @@
       <c r="C97" s="1">
         <v>897670</v>
       </c>
-      <c r="D97" s="11">
+      <c r="D97" s="10">
         <f t="shared" si="5"/>
         <v>-317585</v>
       </c>
-      <c r="E97" s="12">
+      <c r="E97" s="11">
         <f t="shared" si="6"/>
         <v>-0.35378814040794504</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>93</v>
       </c>
@@ -2652,16 +3961,16 @@
       <c r="C98" s="1">
         <v>19870728</v>
       </c>
-      <c r="D98" s="11">
+      <c r="D98" s="10">
         <f t="shared" si="5"/>
         <v>-6326863</v>
       </c>
-      <c r="E98" s="12">
+      <c r="E98" s="11">
         <f t="shared" si="6"/>
         <v>-0.31840116778811528</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>94</v>
       </c>
@@ -2671,16 +3980,16 @@
       <c r="C99" s="1">
         <v>132515</v>
       </c>
-      <c r="D99" s="11">
+      <c r="D99" s="10">
         <f t="shared" si="5"/>
         <v>-126769</v>
       </c>
-      <c r="E99" s="12">
+      <c r="E99" s="11">
         <f t="shared" si="6"/>
         <v>-0.95663887107119949</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>95</v>
       </c>
@@ -2690,16 +3999,16 @@
       <c r="C100" s="1">
         <v>36935</v>
       </c>
-      <c r="D100" s="11">
+      <c r="D100" s="10">
         <f t="shared" si="5"/>
         <v>-36935</v>
       </c>
-      <c r="E100" s="12">
+      <c r="E100" s="11">
         <f t="shared" si="6"/>
         <v>-1</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>96</v>
       </c>
@@ -2709,16 +4018,16 @@
       <c r="C101" s="1">
         <v>29672513</v>
       </c>
-      <c r="D101" s="11">
+      <c r="D101" s="10">
         <f t="shared" si="5"/>
         <v>-8042444</v>
       </c>
-      <c r="E101" s="12">
+      <c r="E101" s="11">
         <f t="shared" si="6"/>
         <v>-0.27104020478481211</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>97</v>
       </c>
@@ -2728,16 +4037,16 @@
       <c r="C102" s="1">
         <v>35986</v>
       </c>
-      <c r="D102" s="11">
+      <c r="D102" s="10">
         <f t="shared" si="5"/>
         <v>-35986</v>
       </c>
-      <c r="E102" s="12">
+      <c r="E102" s="11">
         <f t="shared" si="6"/>
         <v>-1</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>98</v>
       </c>
@@ -2747,16 +4056,16 @@
       <c r="C103" s="1">
         <v>0</v>
       </c>
-      <c r="D103" s="11">
+      <c r="D103" s="10">
         <f t="shared" si="5"/>
         <v>7740</v>
       </c>
-      <c r="E103" s="12" t="str">
+      <c r="E103" s="11" t="str">
         <f t="shared" si="6"/>
         <v>NEW</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>99</v>
       </c>
@@ -2766,16 +4075,16 @@
       <c r="C104" s="1">
         <v>1075001</v>
       </c>
-      <c r="D104" s="11">
+      <c r="D104" s="10">
         <f t="shared" si="5"/>
         <v>-1075001</v>
       </c>
-      <c r="E104" s="12">
+      <c r="E104" s="11">
         <f t="shared" si="6"/>
         <v>-1</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>100</v>
       </c>
@@ -2785,16 +4094,16 @@
       <c r="C105" s="1">
         <v>2428500</v>
       </c>
-      <c r="D105" s="11">
+      <c r="D105" s="10">
         <f t="shared" si="5"/>
         <v>-1165525</v>
       </c>
-      <c r="E105" s="12">
+      <c r="E105" s="11">
         <f t="shared" si="6"/>
         <v>-0.4799361745933704</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>101</v>
       </c>
@@ -2804,16 +4113,16 @@
       <c r="C106" s="1">
         <v>28041</v>
       </c>
-      <c r="D106" s="11">
+      <c r="D106" s="10">
         <f t="shared" si="5"/>
         <v>-28041</v>
       </c>
-      <c r="E106" s="12">
+      <c r="E106" s="11">
         <f t="shared" si="6"/>
         <v>-1</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>102</v>
       </c>
@@ -2823,16 +4132,16 @@
       <c r="C107" s="1">
         <v>6565377</v>
       </c>
-      <c r="D107" s="11">
+      <c r="D107" s="10">
         <f t="shared" si="5"/>
         <v>-2933309</v>
       </c>
-      <c r="E107" s="12">
+      <c r="E107" s="11">
         <f t="shared" si="6"/>
         <v>-0.44678454870146833</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>103</v>
       </c>
@@ -2842,16 +4151,16 @@
       <c r="C108" s="1">
         <v>1635003</v>
       </c>
-      <c r="D108" s="11">
+      <c r="D108" s="10">
         <f t="shared" si="5"/>
         <v>-543313</v>
       </c>
-      <c r="E108" s="12">
+      <c r="E108" s="11">
         <f t="shared" si="6"/>
         <v>-0.3323009193255303</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>104</v>
       </c>
@@ -2861,16 +4170,16 @@
       <c r="C109" s="1">
         <v>1421455</v>
       </c>
-      <c r="D109" s="11">
+      <c r="D109" s="10">
         <f t="shared" si="5"/>
         <v>-739409</v>
       </c>
-      <c r="E109" s="12">
+      <c r="E109" s="11">
         <f t="shared" si="6"/>
         <v>-0.52017756453774477</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>105</v>
       </c>
@@ -2880,16 +4189,16 @@
       <c r="C110" s="1">
         <v>369609</v>
       </c>
-      <c r="D110" s="11">
+      <c r="D110" s="10">
         <f t="shared" si="5"/>
         <v>1687393</v>
       </c>
-      <c r="E110" s="12">
+      <c r="E110" s="11">
         <f t="shared" si="6"/>
         <v>4.5653460819406453</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>106</v>
       </c>
@@ -2899,16 +4208,16 @@
       <c r="C111" s="1">
         <v>21069045</v>
       </c>
-      <c r="D111" s="11">
+      <c r="D111" s="10">
         <f t="shared" si="5"/>
         <v>-9575596</v>
       </c>
-      <c r="E111" s="12">
+      <c r="E111" s="11">
         <f t="shared" si="6"/>
         <v>-0.45448647530061281</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>107</v>
       </c>
@@ -2918,16 +4227,16 @@
       <c r="C112" s="1">
         <v>1915198</v>
       </c>
-      <c r="D112" s="11">
+      <c r="D112" s="10">
         <f t="shared" si="5"/>
         <v>-1552567</v>
       </c>
-      <c r="E112" s="12">
+      <c r="E112" s="11">
         <f t="shared" si="6"/>
         <v>-0.8106561305932859</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>108</v>
       </c>
@@ -2937,16 +4246,16 @@
       <c r="C113" s="1">
         <v>395395</v>
       </c>
-      <c r="D113" s="11">
+      <c r="D113" s="10">
         <f t="shared" si="5"/>
         <v>130887</v>
       </c>
-      <c r="E113" s="12">
+      <c r="E113" s="11">
         <f t="shared" si="6"/>
         <v>0.33102846520568041</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>109</v>
       </c>
@@ -2956,16 +4265,16 @@
       <c r="C114" s="1">
         <v>0</v>
       </c>
-      <c r="D114" s="11">
+      <c r="D114" s="10">
         <f t="shared" si="5"/>
         <v>99385</v>
       </c>
-      <c r="E114" s="12" t="str">
+      <c r="E114" s="11" t="str">
         <f t="shared" si="6"/>
         <v>NEW</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>110</v>
       </c>
@@ -2975,16 +4284,16 @@
       <c r="C115" s="1">
         <v>7482088</v>
       </c>
-      <c r="D115" s="11">
+      <c r="D115" s="10">
         <f t="shared" si="5"/>
         <v>-2346382</v>
       </c>
-      <c r="E115" s="12">
+      <c r="E115" s="11">
         <f t="shared" si="6"/>
         <v>-0.31359989350566314</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>111</v>
       </c>
@@ -2994,16 +4303,16 @@
       <c r="C116" s="1">
         <v>91056</v>
       </c>
-      <c r="D116" s="11">
+      <c r="D116" s="10">
         <f t="shared" si="5"/>
         <v>104944</v>
       </c>
-      <c r="E116" s="12">
+      <c r="E116" s="11">
         <f t="shared" si="6"/>
         <v>1.1525215252152521</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>112</v>
       </c>
@@ -3013,16 +4322,16 @@
       <c r="C117" s="1">
         <v>10739227</v>
       </c>
-      <c r="D117" s="11">
+      <c r="D117" s="10">
         <f t="shared" si="5"/>
         <v>-2212374</v>
       </c>
-      <c r="E117" s="12">
+      <c r="E117" s="11">
         <f t="shared" si="6"/>
         <v>-0.20600868200290393</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>113</v>
       </c>
@@ -3032,16 +4341,16 @@
       <c r="C118" s="1">
         <v>1130404</v>
       </c>
-      <c r="D118" s="11">
+      <c r="D118" s="10">
         <f t="shared" si="5"/>
         <v>-431843</v>
       </c>
-      <c r="E118" s="12">
+      <c r="E118" s="11">
         <f t="shared" si="6"/>
         <v>-0.38202536438299933</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>114</v>
       </c>
@@ -3051,16 +4360,16 @@
       <c r="C119" s="1">
         <v>4779</v>
       </c>
-      <c r="D119" s="11">
+      <c r="D119" s="10">
         <f t="shared" si="5"/>
         <v>-4779</v>
       </c>
-      <c r="E119" s="12">
+      <c r="E119" s="11">
         <f t="shared" si="6"/>
         <v>-1</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>115</v>
       </c>
@@ -3070,16 +4379,16 @@
       <c r="C120" s="1">
         <v>25699820</v>
       </c>
-      <c r="D120" s="11">
+      <c r="D120" s="10">
         <f t="shared" si="5"/>
         <v>-9777973</v>
       </c>
-      <c r="E120" s="12">
+      <c r="E120" s="11">
         <f t="shared" si="6"/>
         <v>-0.38046854024658538</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>116</v>
       </c>
@@ -3089,16 +4398,16 @@
       <c r="C121" s="1">
         <v>68800</v>
       </c>
-      <c r="D121" s="11">
+      <c r="D121" s="10">
         <f t="shared" si="5"/>
         <v>-65250</v>
       </c>
-      <c r="E121" s="12">
+      <c r="E121" s="11">
         <f t="shared" si="6"/>
         <v>-0.94840116279069764</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>117</v>
       </c>
@@ -3108,16 +4417,16 @@
       <c r="C122" s="1">
         <v>2419716</v>
       </c>
-      <c r="D122" s="11">
+      <c r="D122" s="10">
         <f t="shared" si="5"/>
         <v>-1232402</v>
       </c>
-      <c r="E122" s="12">
+      <c r="E122" s="11">
         <f t="shared" si="6"/>
         <v>-0.50931679585538137</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>118</v>
       </c>
@@ -3127,16 +4436,16 @@
       <c r="C123" s="1">
         <v>2408698</v>
       </c>
-      <c r="D123" s="11">
+      <c r="D123" s="10">
         <f t="shared" si="5"/>
         <v>-424245</v>
       </c>
-      <c r="E123" s="12">
+      <c r="E123" s="11">
         <f t="shared" si="6"/>
         <v>-0.1761304239883954</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>119</v>
       </c>
@@ -3146,16 +4455,16 @@
       <c r="C124" s="1">
         <v>75674760</v>
       </c>
-      <c r="D124" s="11">
+      <c r="D124" s="10">
         <f t="shared" si="5"/>
         <v>-7383640</v>
       </c>
-      <c r="E124" s="12">
+      <c r="E124" s="11">
         <f t="shared" si="6"/>
         <v>-9.7570709177009607E-2</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>120</v>
       </c>
@@ -3165,16 +4474,16 @@
       <c r="C125" s="1">
         <v>395859</v>
       </c>
-      <c r="D125" s="11">
+      <c r="D125" s="10">
         <f t="shared" si="5"/>
         <v>180301</v>
       </c>
-      <c r="E125" s="12">
+      <c r="E125" s="11">
         <f t="shared" si="6"/>
         <v>0.4554677296714234</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>121</v>
       </c>
@@ -3184,16 +4493,16 @@
       <c r="C126" s="1">
         <v>22641</v>
       </c>
-      <c r="D126" s="11">
+      <c r="D126" s="10">
         <f t="shared" si="5"/>
         <v>-22641</v>
       </c>
-      <c r="E126" s="12">
+      <c r="E126" s="11">
         <f t="shared" si="6"/>
         <v>-1</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>122</v>
       </c>
@@ -3203,16 +4512,16 @@
       <c r="C127" s="1">
         <v>81554</v>
       </c>
-      <c r="D127" s="11">
+      <c r="D127" s="10">
         <f t="shared" si="5"/>
         <v>7365</v>
       </c>
-      <c r="E127" s="12">
+      <c r="E127" s="11">
         <f t="shared" si="6"/>
         <v>9.030826201044706E-2</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>123</v>
       </c>
@@ -3222,16 +4531,16 @@
       <c r="C128" s="1">
         <v>479898</v>
       </c>
-      <c r="D128" s="11">
+      <c r="D128" s="10">
         <f t="shared" si="5"/>
         <v>-127639</v>
       </c>
-      <c r="E128" s="12">
+      <c r="E128" s="11">
         <f t="shared" si="6"/>
         <v>-0.26597110219254927</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>124</v>
       </c>
@@ -3241,16 +4550,16 @@
       <c r="C129" s="1">
         <v>2473638</v>
       </c>
-      <c r="D129" s="11">
+      <c r="D129" s="10">
         <f t="shared" si="5"/>
         <v>-461221</v>
       </c>
-      <c r="E129" s="12">
+      <c r="E129" s="11">
         <f t="shared" si="6"/>
         <v>-0.18645452568241594</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>125</v>
       </c>
@@ -3260,16 +4569,16 @@
       <c r="C130" s="1">
         <v>10889924</v>
       </c>
-      <c r="D130" s="11">
+      <c r="D130" s="10">
         <f t="shared" si="5"/>
         <v>-4009686</v>
       </c>
-      <c r="E130" s="12">
+      <c r="E130" s="11">
         <f t="shared" si="6"/>
         <v>-0.3682014677053761</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>126</v>
       </c>
@@ -3279,16 +4588,16 @@
       <c r="C131" s="1">
         <v>1290126</v>
       </c>
-      <c r="D131" s="11">
+      <c r="D131" s="10">
         <f t="shared" si="5"/>
         <v>-376123</v>
       </c>
-      <c r="E131" s="12">
+      <c r="E131" s="11">
         <f t="shared" si="6"/>
         <v>-0.29153974107955349</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>127</v>
       </c>
@@ -3298,16 +4607,16 @@
       <c r="C132" s="1">
         <v>2693769</v>
       </c>
-      <c r="D132" s="11">
+      <c r="D132" s="10">
         <f t="shared" si="5"/>
         <v>-604018</v>
       </c>
-      <c r="E132" s="12">
+      <c r="E132" s="11">
         <f t="shared" si="6"/>
         <v>-0.22422783839297283</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>128</v>
       </c>
@@ -3317,16 +4626,16 @@
       <c r="C133" s="1">
         <v>8760</v>
       </c>
-      <c r="D133" s="11">
+      <c r="D133" s="10">
         <f t="shared" si="5"/>
         <v>1845</v>
       </c>
-      <c r="E133" s="12">
+      <c r="E133" s="11">
         <f t="shared" si="6"/>
         <v>0.21061643835616439</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>129</v>
       </c>
@@ -3336,16 +4645,16 @@
       <c r="C134" s="1">
         <v>7800</v>
       </c>
-      <c r="D134" s="11">
+      <c r="D134" s="10">
         <f t="shared" si="5"/>
         <v>-7800</v>
       </c>
-      <c r="E134" s="12">
+      <c r="E134" s="11">
         <f t="shared" si="6"/>
         <v>-1</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>130</v>
       </c>
@@ -3355,16 +4664,16 @@
       <c r="C135" s="1">
         <v>12231</v>
       </c>
-      <c r="D135" s="11">
+      <c r="D135" s="10">
         <f t="shared" si="5"/>
         <v>-6296</v>
       </c>
-      <c r="E135" s="12">
+      <c r="E135" s="11">
         <f t="shared" si="6"/>
         <v>-0.51475758319025422</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>131</v>
       </c>
@@ -3374,16 +4683,16 @@
       <c r="C136" s="1">
         <v>15462991</v>
       </c>
-      <c r="D136" s="11">
+      <c r="D136" s="10">
         <f t="shared" si="5"/>
         <v>-2818751</v>
       </c>
-      <c r="E136" s="12">
+      <c r="E136" s="11">
         <f t="shared" si="6"/>
         <v>-0.18229015330863221</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>132</v>
       </c>
@@ -3393,16 +4702,16 @@
       <c r="C137" s="1">
         <v>12788525</v>
       </c>
-      <c r="D137" s="11">
+      <c r="D137" s="10">
         <f t="shared" si="5"/>
         <v>-3083307</v>
       </c>
-      <c r="E137" s="12">
+      <c r="E137" s="11">
         <f t="shared" si="6"/>
         <v>-0.24109950131074537</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>133</v>
       </c>
@@ -3412,16 +4721,16 @@
       <c r="C138" s="1">
         <v>157863431</v>
       </c>
-      <c r="D138" s="11">
+      <c r="D138" s="10">
         <f t="shared" si="5"/>
         <v>-44018635</v>
       </c>
-      <c r="E138" s="12">
+      <c r="E138" s="11">
         <f t="shared" si="6"/>
         <v>-0.27883997402793048</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>134</v>
       </c>
@@ -3431,16 +4740,16 @@
       <c r="C139" s="1">
         <v>0</v>
       </c>
-      <c r="D139" s="11">
+      <c r="D139" s="10">
         <f t="shared" si="5"/>
         <v>7993</v>
       </c>
-      <c r="E139" s="12" t="str">
+      <c r="E139" s="11" t="str">
         <f t="shared" si="6"/>
         <v>NEW</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>135</v>
       </c>
@@ -3450,16 +4759,16 @@
       <c r="C140" s="1">
         <v>352823</v>
       </c>
-      <c r="D140" s="11">
+      <c r="D140" s="10">
         <f t="shared" si="5"/>
         <v>-284436</v>
       </c>
-      <c r="E140" s="12">
+      <c r="E140" s="11">
         <f t="shared" si="6"/>
         <v>-0.80617193323564507</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>136</v>
       </c>
@@ -3469,16 +4778,16 @@
       <c r="C141" s="1">
         <v>3307725</v>
       </c>
-      <c r="D141" s="11">
+      <c r="D141" s="10">
         <f t="shared" si="5"/>
         <v>536220</v>
       </c>
-      <c r="E141" s="12">
+      <c r="E141" s="11">
         <f t="shared" si="6"/>
         <v>0.16211142099176926</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>137</v>
       </c>
@@ -3488,16 +4797,16 @@
       <c r="C142" s="1">
         <v>133885</v>
       </c>
-      <c r="D142" s="11">
+      <c r="D142" s="10">
         <f t="shared" si="5"/>
         <v>-133885</v>
       </c>
-      <c r="E142" s="12">
+      <c r="E142" s="11">
         <f t="shared" si="6"/>
         <v>-1</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>138</v>
       </c>
@@ -3507,16 +4816,16 @@
       <c r="C143" s="1">
         <v>449503</v>
       </c>
-      <c r="D143" s="11">
+      <c r="D143" s="10">
         <f t="shared" si="5"/>
         <v>1160</v>
       </c>
-      <c r="E143" s="12">
+      <c r="E143" s="11">
         <f t="shared" si="6"/>
         <v>2.5806279379670437E-3</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B144" s="2">
         <f>SUM(B20:B143)</f>
         <v>722755084</v>
@@ -3525,11 +4834,11 @@
         <f>SUM(C20:C143)</f>
         <v>1021250075</v>
       </c>
-      <c r="D144" s="11">
+      <c r="D144" s="10">
         <f t="shared" si="5"/>
         <v>-298494991</v>
       </c>
-      <c r="E144" s="12">
+      <c r="E144" s="11">
         <f t="shared" si="6"/>
         <v>-0.29228393545038417</v>
       </c>
@@ -3540,5 +4849,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
edited data in excel file. added legal protections section.
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -13,8 +13,9 @@
   </bookViews>
   <sheets>
     <sheet name="DISTILLED SPIRITS - VALUE" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -777,6 +778,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-60C8-4E7C-BEE0-2695D84C8E67}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="6"/>
@@ -794,6 +800,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-60C8-4E7C-BEE0-2695D84C8E67}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="7"/>
@@ -811,6 +822,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000F-60C8-4E7C-BEE0-2695D84C8E67}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="8"/>
@@ -831,28 +847,6 @@
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000005-C4AE-4C49-8BA3-064E80B79DED}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="9"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000002-C4AE-4C49-8BA3-064E80B79DED}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -909,8 +903,8 @@
               <c:idx val="2"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="4.3156596794081362E-2"/>
-                  <c:y val="7.3387408265739668E-2"/>
+                  <c:x val="0"/>
+                  <c:y val="9.656237929702588E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:dLblPos val="bestFit"/>
@@ -933,8 +927,8 @@
               <c:idx val="3"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0"/>
-                  <c:y val="9.656237929702588E-2"/>
+                  <c:x val="-3.0114145719454611E-4"/>
+                  <c:y val="8.8837388953263666E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:dLblPos val="bestFit"/>
@@ -957,8 +951,8 @@
               <c:idx val="4"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-2.306021858241826E-2"/>
-                  <c:y val="6.1799922750096561E-2"/>
+                  <c:x val="-2.6715988491574187E-2"/>
+                  <c:y val="3.8624951718811058E-3"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
@@ -966,7 +960,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{34B7A188-D640-43F5-AD43-1C9FB2AB1FCF}" type="CATEGORYNAME">
+                    <a:fld id="{74D07415-98F9-47A7-B405-DF113545CDF4}" type="CATEGORYNAME">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CATEGORY NAME]</a:t>
@@ -974,8 +968,14 @@
                     <a:r>
                       <a:rPr lang="en-US" baseline="0"/>
                       <a:t>
-&lt;1%</a:t>
+&lt;</a:t>
                     </a:r>
+                    <a:fld id="{A0DCCD2E-C8E0-4CF5-B2AF-9E57FE9C7663}" type="PERCENTAGE">
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:pPr/>
+                      <a:t>[PERCENTAGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US" baseline="0"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -998,11 +998,83 @@
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-2.055076037813399E-3"/>
+                  <c:y val="-4.6349942062572348E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000B-60C8-4E7C-BEE0-2695D84C8E67}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0"/>
+                  <c:y val="-5.4074932406334493E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000D-60C8-4E7C-BEE0-2695D84C8E67}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="7"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0"/>
+                  <c:y val="-1.1587485515643106E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000F-60C8-4E7C-BEE0-2695D84C8E67}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
               <c:idx val="8"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-3.904644471845458E-2"/>
-                  <c:y val="-8.8837388953263804E-2"/>
+                  <c:x val="-1.3959387166616504E-2"/>
+                  <c:y val="-6.5732368621940804E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
@@ -1011,44 +1083,9 @@
                   <a:lstStyle/>
                   <a:p>
                     <a:r>
-                      <a:rPr lang="en-US"/>
-                      <a:t>Tequila &lt;1%</a:t>
-                    </a:r>
-                  </a:p>
-                </c:rich>
-              </c:tx>
-              <c:dLblPos val="bestFit"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000005-C4AE-4C49-8BA3-064E80B79DED}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="9"/>
-              <c:layout/>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:r>
-                      <a:rPr lang="en-US"/>
-                      <a:t>Whiskey</a:t>
-                    </a:r>
-                    <a:r>
                       <a:rPr lang="en-US" baseline="0"/>
-                      <a:t>
-</a:t>
+                      <a:t>Tequila
+&lt;</a:t>
                     </a:r>
                     <a:fld id="{688B430C-C531-4E81-B75F-270ED27F49D4}" type="PERCENTAGE">
                       <a:rPr lang="en-US" baseline="0"/>
@@ -1059,7 +1096,7 @@
                   </a:p>
                 </c:rich>
               </c:tx>
-              <c:dLblPos val="outEnd"/>
+              <c:dLblPos val="bestFit"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="1"/>
@@ -1073,7 +1110,7 @@
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000002-C4AE-4C49-8BA3-064E80B79DED}"/>
+                  <c16:uniqueId val="{00000005-C4AE-4C49-8BA3-064E80B79DED}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -1242,7 +1279,6 @@
         <c:custSplit>
           <c:secondPiePt val="0"/>
           <c:secondPiePt val="1"/>
-          <c:secondPiePt val="9"/>
         </c:custSplit>
         <c:secondPieSize val="74"/>
         <c:serLines>
@@ -2172,7 +2208,7 @@
   <dimension ref="A1:H144"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4851,4 +4887,16 @@
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added bourbon boom information and data to excel
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="DISTILLED SPIRITS - VALUE" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="DISTILLED SPIRITS W-KENTUCKY" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="150">
   <si>
     <t>WHISKEY, BOURBON</t>
   </si>
@@ -448,13 +449,41 @@
   </si>
   <si>
     <t>LOST MARKETS</t>
+  </si>
+  <si>
+    <t>KENTUCKY BOURBON</t>
+  </si>
+  <si>
+    <t>OTHER BOURBON</t>
+  </si>
+  <si>
+    <t>OTHER WHISKEY</t>
+  </si>
+  <si>
+    <t>SALES GROWTH</t>
+  </si>
+  <si>
+    <t>YEAR</t>
+  </si>
+  <si>
+    <t>VALUE</t>
+  </si>
+  <si>
+    <t>PREMIUM</t>
+  </si>
+  <si>
+    <t>HIGH END PREMIUM</t>
+  </si>
+  <si>
+    <t>SUPER PREMIUM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
+  <numFmts count="3">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
@@ -516,12 +545,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -545,9 +575,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="3" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
@@ -2207,7 +2242,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H144"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
@@ -4891,12 +4926,215 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B2">
+        <v>2015</v>
+      </c>
+      <c r="C2">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B3" s="13">
+        <f>'DISTILLED SPIRITS - VALUE'!B$3*0.95</f>
+        <v>686617329.79999995</v>
+      </c>
+      <c r="C3" s="13">
+        <f>'DISTILLED SPIRITS - VALUE'!C$3*0.95</f>
+        <v>970881071.25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>142</v>
+      </c>
+      <c r="B4" s="13">
+        <f>'DISTILLED SPIRITS - VALUE'!B$3*0.05</f>
+        <v>36137754.200000003</v>
+      </c>
+      <c r="C4" s="13">
+        <f>'DISTILLED SPIRITS - VALUE'!C$3*0.05</f>
+        <v>51099003.75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>143</v>
+      </c>
+      <c r="B5" s="13">
+        <f>'DISTILLED SPIRITS - VALUE'!B4</f>
+        <v>355497190</v>
+      </c>
+      <c r="C5" s="13">
+        <f>'DISTILLED SPIRITS - VALUE'!C4</f>
+        <v>72225068</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="str">
+        <f>'DISTILLED SPIRITS - VALUE'!A6</f>
+        <v>RUM</v>
+      </c>
+      <c r="B6" s="13">
+        <f>'DISTILLED SPIRITS - VALUE'!B6</f>
+        <v>93158899</v>
+      </c>
+      <c r="C6" s="13">
+        <f>'DISTILLED SPIRITS - VALUE'!C6</f>
+        <v>97457684</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="str">
+        <f>'DISTILLED SPIRITS - VALUE'!A7</f>
+        <v>BRANDY</v>
+      </c>
+      <c r="B7" s="13">
+        <f>'DISTILLED SPIRITS - VALUE'!B7</f>
+        <v>93782350</v>
+      </c>
+      <c r="C7" s="13">
+        <f>'DISTILLED SPIRITS - VALUE'!C7</f>
+        <v>84810485</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="str">
+        <f>'DISTILLED SPIRITS - VALUE'!A8</f>
+        <v>GIN</v>
+      </c>
+      <c r="B8" s="13">
+        <f>'DISTILLED SPIRITS - VALUE'!B8</f>
+        <v>6884192</v>
+      </c>
+      <c r="C8" s="13">
+        <f>'DISTILLED SPIRITS - VALUE'!C8</f>
+        <v>4907460</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="str">
+        <f>'DISTILLED SPIRITS - VALUE'!A9</f>
+        <v>VODKA</v>
+      </c>
+      <c r="B9" s="13">
+        <f>'DISTILLED SPIRITS - VALUE'!B9</f>
+        <v>63622174</v>
+      </c>
+      <c r="C9" s="13">
+        <f>'DISTILLED SPIRITS - VALUE'!C9</f>
+        <v>51000009</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="str">
+        <f>'DISTILLED SPIRITS - VALUE'!A10</f>
+        <v>CORDIALS</v>
+      </c>
+      <c r="B10" s="13">
+        <f>'DISTILLED SPIRITS - VALUE'!B10</f>
+        <v>90663881</v>
+      </c>
+      <c r="C10" s="13">
+        <f>'DISTILLED SPIRITS - VALUE'!C10</f>
+        <v>89408273</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="str">
+        <f>'DISTILLED SPIRITS - VALUE'!A11</f>
+        <v>OTHER DISTILLED SPIRITS</v>
+      </c>
+      <c r="B11" s="13">
+        <f>'DISTILLED SPIRITS - VALUE'!B11</f>
+        <v>138492124</v>
+      </c>
+      <c r="C11" s="13">
+        <f>'DISTILLED SPIRITS - VALUE'!C11</f>
+        <v>139856150</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="str">
+        <f>'DISTILLED SPIRITS - VALUE'!A12</f>
+        <v>TEQUILA</v>
+      </c>
+      <c r="B12" s="13">
+        <f>'DISTILLED SPIRITS - VALUE'!B12</f>
+        <v>5621518</v>
+      </c>
+      <c r="C12" s="13">
+        <f>'DISTILLED SPIRITS - VALUE'!C12</f>
+        <v>6651931</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D1" t="s">
+        <v>148</v>
+      </c>
+      <c r="E1" t="s">
+        <v>149</v>
+      </c>
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
more data. entering post boom data.
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
   </bookViews>
   <sheets>
     <sheet name="DISTILLED SPIRITS - VALUE" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="179">
   <si>
     <t>WHISKEY, BOURBON</t>
   </si>
@@ -557,6 +557,21 @@
   </si>
   <si>
     <t>Sum</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>2015</t>
+  </si>
+  <si>
+    <t>2014</t>
+  </si>
+  <si>
+    <t>TOP 10 BOURBON IMPORTERS 2014</t>
+  </si>
+  <si>
+    <t>TOP 10 BOURBON IMPORTERS 2015</t>
   </si>
 </sst>
 </file>
@@ -570,7 +585,7 @@
     <numFmt numFmtId="168" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="169" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -602,21 +617,41 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -681,6 +716,61 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -688,7 +778,7 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -749,7 +839,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -761,8 +851,29 @@
     <xf numFmtId="168" fontId="0" fillId="0" borderId="4" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -771,7 +882,65 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -8042,6 +8211,27 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A19:E143" totalsRowShown="0">
+  <autoFilter ref="A19:E143"/>
+  <sortState ref="A20:E143">
+    <sortCondition descending="1" ref="B19:B143"/>
+  </sortState>
+  <tableColumns count="5">
+    <tableColumn id="1" name="Column1"/>
+    <tableColumn id="2" name="2015" dataDxfId="3" dataCellStyle="Comma"/>
+    <tableColumn id="3" name="2014" dataDxfId="2" dataCellStyle="Comma"/>
+    <tableColumn id="4" name="$ CHANGE" dataDxfId="1">
+      <calculatedColumnFormula>B20-C20</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" name="% CHANGE" dataDxfId="0" dataCellStyle="Percent">
+      <calculatedColumnFormula>IF(C20=0,"NEW",D20/C20)</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -8305,10 +8495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H144"/>
+  <dimension ref="A1:K144"/>
   <sheetViews>
-    <sheetView topLeftCell="A124" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="G61" sqref="G61:K72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8316,8 +8506,10 @@
     <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" customWidth="1"/>
     <col min="7" max="8" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.35">
@@ -8577,12 +8769,15 @@
         <v>1.3902181872573343E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B19">
-        <v>2015</v>
-      </c>
-      <c r="C19">
-        <v>2014</v>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>174</v>
+      </c>
+      <c r="B19" t="s">
+        <v>175</v>
+      </c>
+      <c r="C19" t="s">
+        <v>176</v>
       </c>
       <c r="D19" t="s">
         <v>12</v>
@@ -8597,23 +8792,23 @@
         <v>140</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>15</v>
+        <v>133</v>
       </c>
       <c r="B20" s="1">
-        <v>0</v>
+        <v>113844796</v>
       </c>
       <c r="C20" s="1">
-        <v>153007</v>
+        <v>157863431</v>
       </c>
       <c r="D20" s="10">
-        <f t="shared" ref="D20" si="2">B20-C20</f>
-        <v>-153007</v>
+        <f>B20-C20</f>
+        <v>-44018635</v>
       </c>
       <c r="E20" s="11">
         <f>IF(C20=0,"NEW",D20/C20)</f>
-        <v>-1</v>
+        <v>-0.27883997402793048</v>
       </c>
       <c r="G20">
         <f>COUNTIF($E$20:$E$144, "NEW")</f>
@@ -8624,2341 +8819,2781 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>16</v>
+        <v>76</v>
       </c>
       <c r="B21" s="1">
-        <v>0</v>
+        <v>72746897</v>
       </c>
       <c r="C21" s="1">
-        <v>115461</v>
+        <v>72882617</v>
       </c>
       <c r="D21" s="10">
-        <f t="shared" ref="D21:D84" si="3">B21-C21</f>
-        <v>-115461</v>
+        <f>B21-C21</f>
+        <v>-135720</v>
       </c>
       <c r="E21" s="11">
-        <f t="shared" ref="E21:E84" si="4">IF(C21=0,"NEW",D21/C21)</f>
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+        <f>IF(C21=0,"NEW",D21/C21)</f>
+        <v>-1.862172429949929E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B22" s="1">
-        <v>52839</v>
+        <v>70425166</v>
       </c>
       <c r="C22" s="1">
-        <v>47349</v>
+        <v>102812427</v>
       </c>
       <c r="D22" s="10">
-        <f t="shared" si="3"/>
-        <v>5490</v>
+        <f>B22-C22</f>
+        <v>-32387261</v>
       </c>
       <c r="E22" s="11">
-        <f t="shared" si="4"/>
-        <v>0.11594753849078122</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+        <f>IF(C22=0,"NEW",D22/C22)</f>
+        <v>-0.31501309661720173</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>119</v>
+      </c>
+      <c r="B23" s="1">
+        <v>68291120</v>
+      </c>
+      <c r="C23" s="1">
+        <v>75674760</v>
+      </c>
+      <c r="D23" s="10">
+        <f>B23-C23</f>
+        <v>-7383640</v>
+      </c>
+      <c r="E23" s="11">
+        <f>IF(C23=0,"NEW",D23/C23)</f>
+        <v>-9.7570709177009607E-2</v>
+      </c>
+      <c r="H23" s="14"/>
+      <c r="I23" s="14"/>
+      <c r="J23" s="14"/>
+      <c r="K23" s="14"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>57</v>
+      </c>
+      <c r="B24" s="1">
+        <v>52081663</v>
+      </c>
+      <c r="C24" s="1">
+        <v>101571505</v>
+      </c>
+      <c r="D24" s="10">
+        <f>B24-C24</f>
+        <v>-49489842</v>
+      </c>
+      <c r="E24" s="11">
+        <f>IF(C24=0,"NEW",D24/C24)</f>
+        <v>-0.48724139708277436</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>59</v>
+      </c>
+      <c r="B25" s="1">
+        <v>50849324</v>
+      </c>
+      <c r="C25" s="1">
+        <v>96610083</v>
+      </c>
+      <c r="D25" s="10">
+        <f>B25-C25</f>
+        <v>-45760759</v>
+      </c>
+      <c r="E25" s="11">
+        <f>IF(C25=0,"NEW",D25/C25)</f>
+        <v>-0.47366442072097176</v>
+      </c>
+      <c r="I25" s="24"/>
+      <c r="J25" s="24"/>
+      <c r="K25" s="3"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>36</v>
+      </c>
+      <c r="B26" s="1">
+        <v>34292071</v>
+      </c>
+      <c r="C26" s="1">
+        <v>33423004</v>
+      </c>
+      <c r="D26" s="10">
+        <f>B26-C26</f>
+        <v>869067</v>
+      </c>
+      <c r="E26" s="11">
+        <f>IF(C26=0,"NEW",D26/C26)</f>
+        <v>2.6002061334762131E-2</v>
+      </c>
+      <c r="I26" s="24"/>
+      <c r="J26" s="24"/>
+      <c r="K26" s="3"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>81</v>
+      </c>
+      <c r="B27" s="1">
+        <v>30965147</v>
+      </c>
+      <c r="C27" s="1">
+        <v>23501652</v>
+      </c>
+      <c r="D27" s="10">
+        <f>B27-C27</f>
+        <v>7463495</v>
+      </c>
+      <c r="E27" s="11">
+        <f>IF(C27=0,"NEW",D27/C27)</f>
+        <v>0.31757320719411553</v>
+      </c>
+      <c r="I27" s="24"/>
+      <c r="J27" s="24"/>
+      <c r="K27" s="3"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>96</v>
+      </c>
+      <c r="B28" s="1">
+        <v>21630069</v>
+      </c>
+      <c r="C28" s="1">
+        <v>29672513</v>
+      </c>
+      <c r="D28" s="10">
+        <f>B28-C28</f>
+        <v>-8042444</v>
+      </c>
+      <c r="E28" s="11">
+        <f>IF(C28=0,"NEW",D28/C28)</f>
+        <v>-0.27104020478481211</v>
+      </c>
+      <c r="I28" s="24"/>
+      <c r="J28" s="24"/>
+      <c r="K28" s="3"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>115</v>
+      </c>
+      <c r="B29" s="1">
+        <v>15921847</v>
+      </c>
+      <c r="C29" s="1">
+        <v>25699820</v>
+      </c>
+      <c r="D29" s="10">
+        <f>B29-C29</f>
+        <v>-9777973</v>
+      </c>
+      <c r="E29" s="11">
+        <f>IF(C29=0,"NEW",D29/C29)</f>
+        <v>-0.38046854024658538</v>
+      </c>
+      <c r="I29" s="24"/>
+      <c r="J29" s="24"/>
+      <c r="K29" s="3"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>74</v>
+      </c>
+      <c r="B30" s="1">
+        <v>14348603</v>
+      </c>
+      <c r="C30" s="1">
+        <v>27439305</v>
+      </c>
+      <c r="D30" s="10">
+        <f>B30-C30</f>
+        <v>-13090702</v>
+      </c>
+      <c r="E30" s="11">
+        <f>IF(C30=0,"NEW",D30/C30)</f>
+        <v>-0.4770784828551598</v>
+      </c>
+      <c r="I30" s="24"/>
+      <c r="J30" s="24"/>
+      <c r="K30" s="3"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>93</v>
+      </c>
+      <c r="B31" s="1">
+        <v>13543865</v>
+      </c>
+      <c r="C31" s="1">
+        <v>19870728</v>
+      </c>
+      <c r="D31" s="10">
+        <f>B31-C31</f>
+        <v>-6326863</v>
+      </c>
+      <c r="E31" s="11">
+        <f>IF(C31=0,"NEW",D31/C31)</f>
+        <v>-0.31840116778811528</v>
+      </c>
+      <c r="I31" s="24"/>
+      <c r="J31" s="24"/>
+      <c r="K31" s="3"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>131</v>
+      </c>
+      <c r="B32" s="1">
+        <v>12644240</v>
+      </c>
+      <c r="C32" s="1">
+        <v>15462991</v>
+      </c>
+      <c r="D32" s="10">
+        <f>B32-C32</f>
+        <v>-2818751</v>
+      </c>
+      <c r="E32" s="11">
+        <f>IF(C32=0,"NEW",D32/C32)</f>
+        <v>-0.18229015330863221</v>
+      </c>
+      <c r="I32" s="24"/>
+      <c r="J32" s="24"/>
+      <c r="K32" s="3"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>106</v>
+      </c>
+      <c r="B33" s="1">
+        <v>11493449</v>
+      </c>
+      <c r="C33" s="1">
+        <v>21069045</v>
+      </c>
+      <c r="D33" s="10">
+        <f>B33-C33</f>
+        <v>-9575596</v>
+      </c>
+      <c r="E33" s="11">
+        <f>IF(C33=0,"NEW",D33/C33)</f>
+        <v>-0.45448647530061281</v>
+      </c>
+      <c r="I33" s="24"/>
+      <c r="J33" s="24"/>
+      <c r="K33" s="3"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>27</v>
+      </c>
+      <c r="B34" s="1">
+        <v>10908743</v>
+      </c>
+      <c r="C34" s="1">
+        <v>18660355</v>
+      </c>
+      <c r="D34" s="10">
+        <f>B34-C34</f>
+        <v>-7751612</v>
+      </c>
+      <c r="E34" s="11">
+        <f>IF(C34=0,"NEW",D34/C34)</f>
+        <v>-0.41540538751808315</v>
+      </c>
+      <c r="I34" s="24"/>
+      <c r="J34" s="24"/>
+      <c r="K34" s="3"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>132</v>
+      </c>
+      <c r="B35" s="1">
+        <v>9705218</v>
+      </c>
+      <c r="C35" s="1">
+        <v>12788525</v>
+      </c>
+      <c r="D35" s="10">
+        <f>B35-C35</f>
+        <v>-3083307</v>
+      </c>
+      <c r="E35" s="11">
+        <f>IF(C35=0,"NEW",D35/C35)</f>
+        <v>-0.24109950131074537</v>
+      </c>
+      <c r="H35" s="46"/>
+      <c r="I35" s="46"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>90</v>
+      </c>
+      <c r="B36" s="1">
+        <v>8684806</v>
+      </c>
+      <c r="C36" s="1">
+        <v>10043085</v>
+      </c>
+      <c r="D36" s="10">
+        <f>B36-C36</f>
+        <v>-1358279</v>
+      </c>
+      <c r="E36" s="11">
+        <f>IF(C36=0,"NEW",D36/C36)</f>
+        <v>-0.13524519607272067</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>112</v>
+      </c>
+      <c r="B37" s="1">
+        <v>8526853</v>
+      </c>
+      <c r="C37" s="1">
+        <v>10739227</v>
+      </c>
+      <c r="D37" s="10">
+        <f>B37-C37</f>
+        <v>-2212374</v>
+      </c>
+      <c r="E37" s="11">
+        <f>IF(C37=0,"NEW",D37/C37)</f>
+        <v>-0.20600868200290393</v>
+      </c>
+      <c r="H37" s="35"/>
+      <c r="I37" s="36"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>125</v>
+      </c>
+      <c r="B38" s="1">
+        <v>6880238</v>
+      </c>
+      <c r="C38" s="1">
+        <v>10889924</v>
+      </c>
+      <c r="D38" s="10">
+        <f>B38-C38</f>
+        <v>-4009686</v>
+      </c>
+      <c r="E38" s="11">
+        <f>IF(C38=0,"NEW",D38/C38)</f>
+        <v>-0.3682014677053761</v>
+      </c>
+      <c r="H38" s="39"/>
+      <c r="I38" s="40"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>38</v>
+      </c>
+      <c r="B39" s="1">
+        <v>6714270</v>
+      </c>
+      <c r="C39" s="1">
+        <v>12390236</v>
+      </c>
+      <c r="D39" s="10">
+        <f>B39-C39</f>
+        <v>-5675966</v>
+      </c>
+      <c r="E39" s="11">
+        <f>IF(C39=0,"NEW",D39/C39)</f>
+        <v>-0.45809991028419472</v>
+      </c>
+      <c r="H39" s="35"/>
+      <c r="I39" s="36"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>32</v>
+      </c>
+      <c r="B40" s="1">
+        <v>5458628</v>
+      </c>
+      <c r="C40" s="1">
+        <v>6987958</v>
+      </c>
+      <c r="D40" s="10">
+        <f>B40-C40</f>
+        <v>-1529330</v>
+      </c>
+      <c r="E40" s="11">
+        <f>IF(C40=0,"NEW",D40/C40)</f>
+        <v>-0.21885220260339286</v>
+      </c>
+      <c r="H40" s="39"/>
+      <c r="I40" s="40"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>110</v>
+      </c>
+      <c r="B41" s="1">
+        <v>5135706</v>
+      </c>
+      <c r="C41" s="1">
+        <v>7482088</v>
+      </c>
+      <c r="D41" s="10">
+        <f>B41-C41</f>
+        <v>-2346382</v>
+      </c>
+      <c r="E41" s="11">
+        <f>IF(C41=0,"NEW",D41/C41)</f>
+        <v>-0.31359989350566314</v>
+      </c>
+      <c r="H41" s="35"/>
+      <c r="I41" s="36"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>58</v>
+      </c>
+      <c r="B42" s="1">
+        <v>5062153</v>
+      </c>
+      <c r="C42" s="1">
+        <v>7788444</v>
+      </c>
+      <c r="D42" s="10">
+        <f>B42-C42</f>
+        <v>-2726291</v>
+      </c>
+      <c r="E42" s="11">
+        <f>IF(C42=0,"NEW",D42/C42)</f>
+        <v>-0.35004308947974716</v>
+      </c>
+      <c r="H42" s="39"/>
+      <c r="I42" s="40"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>39</v>
+      </c>
+      <c r="B43" s="1">
+        <v>4170090</v>
+      </c>
+      <c r="C43" s="1">
+        <v>4467702</v>
+      </c>
+      <c r="D43" s="10">
+        <f>B43-C43</f>
+        <v>-297612</v>
+      </c>
+      <c r="E43" s="11">
+        <f>IF(C43=0,"NEW",D43/C43)</f>
+        <v>-6.6614111684261845E-2</v>
+      </c>
+      <c r="H43" s="35"/>
+      <c r="I43" s="36"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>33</v>
+      </c>
+      <c r="B44" s="1">
+        <v>3895474</v>
+      </c>
+      <c r="C44" s="1">
+        <v>6402257</v>
+      </c>
+      <c r="D44" s="10">
+        <f>B44-C44</f>
+        <v>-2506783</v>
+      </c>
+      <c r="E44" s="11">
+        <f>IF(C44=0,"NEW",D44/C44)</f>
+        <v>-0.39154676233709457</v>
+      </c>
+      <c r="H44" s="39"/>
+      <c r="I44" s="40"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>136</v>
+      </c>
+      <c r="B45" s="1">
+        <v>3843945</v>
+      </c>
+      <c r="C45" s="1">
+        <v>3307725</v>
+      </c>
+      <c r="D45" s="10">
+        <f>B45-C45</f>
+        <v>536220</v>
+      </c>
+      <c r="E45" s="11">
+        <f>IF(C45=0,"NEW",D45/C45)</f>
+        <v>0.16211142099176926</v>
+      </c>
+      <c r="H45" s="35"/>
+      <c r="I45" s="36"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>102</v>
+      </c>
+      <c r="B46" s="1">
+        <v>3632068</v>
+      </c>
+      <c r="C46" s="1">
+        <v>6565377</v>
+      </c>
+      <c r="D46" s="10">
+        <f>B46-C46</f>
+        <v>-2933309</v>
+      </c>
+      <c r="E46" s="11">
+        <f>IF(C46=0,"NEW",D46/C46)</f>
+        <v>-0.44678454870146833</v>
+      </c>
+      <c r="H46" s="39"/>
+      <c r="I46" s="40"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>21</v>
+      </c>
+      <c r="B47" s="1">
+        <v>3613527</v>
+      </c>
+      <c r="C47" s="1">
+        <v>7795106</v>
+      </c>
+      <c r="D47" s="10">
+        <f>B47-C47</f>
+        <v>-4181579</v>
+      </c>
+      <c r="E47" s="11">
+        <f>IF(C47=0,"NEW",D47/C47)</f>
+        <v>-0.53643645128109863</v>
+      </c>
+      <c r="G47" s="47" t="s">
+        <v>177</v>
+      </c>
+      <c r="H47" s="47"/>
+      <c r="I47" s="47"/>
+      <c r="J47" s="47"/>
+      <c r="K47" s="47"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>83</v>
+      </c>
+      <c r="B48" s="1">
+        <v>2745172</v>
+      </c>
+      <c r="C48" s="1">
+        <v>4125306</v>
+      </c>
+      <c r="D48" s="10">
+        <f>B48-C48</f>
+        <v>-1380134</v>
+      </c>
+      <c r="E48" s="11">
+        <f>IF(C48=0,"NEW",D48/C48)</f>
+        <v>-0.33455312163509809</v>
+      </c>
+      <c r="G48" s="43" t="s">
+        <v>159</v>
+      </c>
+      <c r="H48" s="44" t="s">
+        <v>175</v>
+      </c>
+      <c r="I48" s="44" t="s">
+        <v>176</v>
+      </c>
+      <c r="J48" s="44" t="s">
+        <v>12</v>
+      </c>
+      <c r="K48" s="45" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>72</v>
+      </c>
+      <c r="B49" s="1">
+        <v>2585959</v>
+      </c>
+      <c r="C49" s="1">
+        <v>4075159</v>
+      </c>
+      <c r="D49" s="10">
+        <f>B49-C49</f>
+        <v>-1489200</v>
+      </c>
+      <c r="E49" s="11">
+        <f>IF(C49=0,"NEW",D49/C49)</f>
+        <v>-0.36543359412479365</v>
+      </c>
+      <c r="G49" s="35" t="s">
+        <v>133</v>
+      </c>
+      <c r="H49" s="36">
+        <v>113844796</v>
+      </c>
+      <c r="I49" s="36">
+        <v>157863431</v>
+      </c>
+      <c r="J49" s="37">
+        <f>H49-I49</f>
+        <v>-44018635</v>
+      </c>
+      <c r="K49" s="38">
+        <f>IF(I49=0,"NEW",J49/I49)</f>
+        <v>-0.27883997402793048</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>73</v>
+      </c>
+      <c r="B50" s="1">
+        <v>2576157</v>
+      </c>
+      <c r="C50" s="1">
+        <v>3406976</v>
+      </c>
+      <c r="D50" s="10">
+        <f>B50-C50</f>
+        <v>-830819</v>
+      </c>
+      <c r="E50" s="11">
+        <f>IF(C50=0,"NEW",D50/C50)</f>
+        <v>-0.24385818978472404</v>
+      </c>
+      <c r="G50" s="39" t="s">
+        <v>20</v>
+      </c>
+      <c r="H50" s="40">
+        <v>70425166</v>
+      </c>
+      <c r="I50" s="40">
+        <v>102812427</v>
+      </c>
+      <c r="J50" s="41">
+        <f>H50-I50</f>
+        <v>-32387261</v>
+      </c>
+      <c r="K50" s="42">
+        <f>IF(I50=0,"NEW",J50/I50)</f>
+        <v>-0.31501309661720173</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>60</v>
+      </c>
+      <c r="B51" s="1">
+        <v>2384085</v>
+      </c>
+      <c r="C51" s="1">
+        <v>9798667</v>
+      </c>
+      <c r="D51" s="10">
+        <f>B51-C51</f>
+        <v>-7414582</v>
+      </c>
+      <c r="E51" s="11">
+        <f>IF(C51=0,"NEW",D51/C51)</f>
+        <v>-0.75669292568060531</v>
+      </c>
+      <c r="G51" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="H51" s="36">
+        <v>52081663</v>
+      </c>
+      <c r="I51" s="36">
+        <v>101571505</v>
+      </c>
+      <c r="J51" s="37">
+        <f>H51-I51</f>
+        <v>-49489842</v>
+      </c>
+      <c r="K51" s="38">
+        <f>IF(I51=0,"NEW",J51/I51)</f>
+        <v>-0.48724139708277436</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>80</v>
+      </c>
+      <c r="B52" s="1">
+        <v>2333826</v>
+      </c>
+      <c r="C52" s="1">
+        <v>2826572</v>
+      </c>
+      <c r="D52" s="10">
+        <f>B52-C52</f>
+        <v>-492746</v>
+      </c>
+      <c r="E52" s="11">
+        <f>IF(C52=0,"NEW",D52/C52)</f>
+        <v>-0.17432635715630099</v>
+      </c>
+      <c r="G52" s="39" t="s">
+        <v>59</v>
+      </c>
+      <c r="H52" s="40">
+        <v>50849324</v>
+      </c>
+      <c r="I52" s="40">
+        <v>96610083</v>
+      </c>
+      <c r="J52" s="41">
+        <f>H52-I52</f>
+        <v>-45760759</v>
+      </c>
+      <c r="K52" s="42">
+        <f>IF(I52=0,"NEW",J52/I52)</f>
+        <v>-0.47366442072097176</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>43</v>
+      </c>
+      <c r="B53" s="1">
+        <v>2125328</v>
+      </c>
+      <c r="C53" s="1">
+        <v>3743552</v>
+      </c>
+      <c r="D53" s="10">
+        <f>B53-C53</f>
+        <v>-1618224</v>
+      </c>
+      <c r="E53" s="11">
+        <f>IF(C53=0,"NEW",D53/C53)</f>
+        <v>-0.43226967329424032</v>
+      </c>
+      <c r="G53" s="35" t="s">
+        <v>119</v>
+      </c>
+      <c r="H53" s="36">
+        <v>68291120</v>
+      </c>
+      <c r="I53" s="36">
+        <v>75674760</v>
+      </c>
+      <c r="J53" s="37">
+        <f>H53-I53</f>
+        <v>-7383640</v>
+      </c>
+      <c r="K53" s="38">
+        <f>IF(I53=0,"NEW",J53/I53)</f>
+        <v>-9.7570709177009607E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>127</v>
+      </c>
+      <c r="B54" s="1">
+        <v>2089751</v>
+      </c>
+      <c r="C54" s="1">
+        <v>2693769</v>
+      </c>
+      <c r="D54" s="10">
+        <f>B54-C54</f>
+        <v>-604018</v>
+      </c>
+      <c r="E54" s="11">
+        <f>IF(C54=0,"NEW",D54/C54)</f>
+        <v>-0.22422783839297283</v>
+      </c>
+      <c r="G54" s="39" t="s">
+        <v>76</v>
+      </c>
+      <c r="H54" s="40">
+        <v>72746897</v>
+      </c>
+      <c r="I54" s="40">
+        <v>72882617</v>
+      </c>
+      <c r="J54" s="41">
+        <f>H54-I54</f>
+        <v>-135720</v>
+      </c>
+      <c r="K54" s="42">
+        <f>IF(I54=0,"NEW",J54/I54)</f>
+        <v>-1.862172429949929E-3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>105</v>
+      </c>
+      <c r="B55" s="1">
+        <v>2057002</v>
+      </c>
+      <c r="C55" s="1">
+        <v>369609</v>
+      </c>
+      <c r="D55" s="10">
+        <f>B55-C55</f>
+        <v>1687393</v>
+      </c>
+      <c r="E55" s="11">
+        <f>IF(C55=0,"NEW",D55/C55)</f>
+        <v>4.5653460819406453</v>
+      </c>
+      <c r="G55" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="H55" s="36">
+        <v>34292071</v>
+      </c>
+      <c r="I55" s="36">
+        <v>33423004</v>
+      </c>
+      <c r="J55" s="37">
+        <f>H55-I55</f>
+        <v>869067</v>
+      </c>
+      <c r="K55" s="38">
+        <f>IF(I55=0,"NEW",J55/I55)</f>
+        <v>2.6002061334762131E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>54</v>
+      </c>
+      <c r="B56" s="1">
+        <v>2044602</v>
+      </c>
+      <c r="C56" s="1">
+        <v>2802152</v>
+      </c>
+      <c r="D56" s="10">
+        <f>B56-C56</f>
+        <v>-757550</v>
+      </c>
+      <c r="E56" s="11">
+        <f>IF(C56=0,"NEW",D56/C56)</f>
+        <v>-0.27034579137748416</v>
+      </c>
+      <c r="G56" s="39" t="s">
+        <v>96</v>
+      </c>
+      <c r="H56" s="40">
+        <v>21630069</v>
+      </c>
+      <c r="I56" s="40">
+        <v>29672513</v>
+      </c>
+      <c r="J56" s="41">
+        <f>H56-I56</f>
+        <v>-8042444</v>
+      </c>
+      <c r="K56" s="42">
+        <f>IF(I56=0,"NEW",J56/I56)</f>
+        <v>-0.27104020478481211</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>124</v>
+      </c>
+      <c r="B57" s="1">
+        <v>2012417</v>
+      </c>
+      <c r="C57" s="1">
+        <v>2473638</v>
+      </c>
+      <c r="D57" s="10">
+        <f>B57-C57</f>
+        <v>-461221</v>
+      </c>
+      <c r="E57" s="11">
+        <f>IF(C57=0,"NEW",D57/C57)</f>
+        <v>-0.18645452568241594</v>
+      </c>
+      <c r="G57" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="H57" s="36">
+        <v>14348603</v>
+      </c>
+      <c r="I57" s="36">
+        <v>27439305</v>
+      </c>
+      <c r="J57" s="37">
+        <f>H57-I57</f>
+        <v>-13090702</v>
+      </c>
+      <c r="K57" s="38">
+        <f>IF(I57=0,"NEW",J57/I57)</f>
+        <v>-0.4770784828551598</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>70</v>
+      </c>
+      <c r="B58" s="1">
+        <v>1985216</v>
+      </c>
+      <c r="C58" s="1">
+        <v>3582648</v>
+      </c>
+      <c r="D58" s="10">
+        <f>B58-C58</f>
+        <v>-1597432</v>
+      </c>
+      <c r="E58" s="11">
+        <f>IF(C58=0,"NEW",D58/C58)</f>
+        <v>-0.44588025393507819</v>
+      </c>
+      <c r="G58" s="39" t="s">
+        <v>115</v>
+      </c>
+      <c r="H58" s="40">
+        <v>15921847</v>
+      </c>
+      <c r="I58" s="40">
+        <v>25699820</v>
+      </c>
+      <c r="J58" s="41">
+        <f>H58-I58</f>
+        <v>-9777973</v>
+      </c>
+      <c r="K58" s="42">
+        <f>IF(I58=0,"NEW",J58/I58)</f>
+        <v>-0.38046854024658538</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>118</v>
+      </c>
+      <c r="B59" s="1">
+        <v>1984453</v>
+      </c>
+      <c r="C59" s="1">
+        <v>2408698</v>
+      </c>
+      <c r="D59" s="10">
+        <f>B59-C59</f>
+        <v>-424245</v>
+      </c>
+      <c r="E59" s="11">
+        <f>IF(C59=0,"NEW",D59/C59)</f>
+        <v>-0.1761304239883954</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>29</v>
+      </c>
+      <c r="B60" s="1">
+        <v>1837345</v>
+      </c>
+      <c r="C60" s="1">
+        <v>5302363</v>
+      </c>
+      <c r="D60" s="10">
+        <f>B60-C60</f>
+        <v>-3465018</v>
+      </c>
+      <c r="E60" s="11">
+        <f>IF(C60=0,"NEW",D60/C60)</f>
+        <v>-0.65348562518258368</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>47</v>
+      </c>
+      <c r="B61" s="1">
+        <v>1786170</v>
+      </c>
+      <c r="C61" s="1">
+        <v>2284321</v>
+      </c>
+      <c r="D61" s="10">
+        <f>B61-C61</f>
+        <v>-498151</v>
+      </c>
+      <c r="E61" s="11">
+        <f>IF(C61=0,"NEW",D61/C61)</f>
+        <v>-0.21807399222788743</v>
+      </c>
+      <c r="G61" s="47" t="s">
+        <v>178</v>
+      </c>
+      <c r="H61" s="47"/>
+      <c r="I61" s="47"/>
+      <c r="J61" s="47"/>
+      <c r="K61" s="47"/>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>67</v>
+      </c>
+      <c r="B62" s="1">
+        <v>1615940</v>
+      </c>
+      <c r="C62" s="1">
+        <v>2232330</v>
+      </c>
+      <c r="D62" s="10">
+        <f>B62-C62</f>
+        <v>-616390</v>
+      </c>
+      <c r="E62" s="11">
+        <f>IF(C62=0,"NEW",D62/C62)</f>
+        <v>-0.27611957013523986</v>
+      </c>
+      <c r="G62" s="43" t="s">
+        <v>159</v>
+      </c>
+      <c r="H62" s="44" t="s">
+        <v>175</v>
+      </c>
+      <c r="I62" s="44" t="s">
+        <v>176</v>
+      </c>
+      <c r="J62" s="44" t="s">
+        <v>12</v>
+      </c>
+      <c r="K62" s="45" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>100</v>
+      </c>
+      <c r="B63" s="1">
+        <v>1262975</v>
+      </c>
+      <c r="C63" s="1">
+        <v>2428500</v>
+      </c>
+      <c r="D63" s="10">
+        <f>B63-C63</f>
+        <v>-1165525</v>
+      </c>
+      <c r="E63" s="11">
+        <f>IF(C63=0,"NEW",D63/C63)</f>
+        <v>-0.4799361745933704</v>
+      </c>
+      <c r="G63" s="35" t="s">
+        <v>133</v>
+      </c>
+      <c r="H63" s="36">
+        <v>113844796</v>
+      </c>
+      <c r="I63" s="36">
+        <v>157863431</v>
+      </c>
+      <c r="J63" s="37">
+        <f>H63-I63</f>
+        <v>-44018635</v>
+      </c>
+      <c r="K63" s="38">
+        <f>IF(I63=0,"NEW",J63/I63)</f>
+        <v>-0.27883997402793048</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>117</v>
+      </c>
+      <c r="B64" s="1">
+        <v>1187314</v>
+      </c>
+      <c r="C64" s="1">
+        <v>2419716</v>
+      </c>
+      <c r="D64" s="10">
+        <f>B64-C64</f>
+        <v>-1232402</v>
+      </c>
+      <c r="E64" s="11">
+        <f>IF(C64=0,"NEW",D64/C64)</f>
+        <v>-0.50931679585538137</v>
+      </c>
+      <c r="G64" s="39" t="s">
+        <v>76</v>
+      </c>
+      <c r="H64" s="40">
+        <v>72746897</v>
+      </c>
+      <c r="I64" s="40">
+        <v>72882617</v>
+      </c>
+      <c r="J64" s="41">
+        <f>H64-I64</f>
+        <v>-135720</v>
+      </c>
+      <c r="K64" s="42">
+        <f>IF(I64=0,"NEW",J64/I64)</f>
+        <v>-1.862172429949929E-3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>68</v>
+      </c>
+      <c r="B65" s="1">
+        <v>1158921</v>
+      </c>
+      <c r="C65" s="1">
+        <v>2295573</v>
+      </c>
+      <c r="D65" s="10">
+        <f>B65-C65</f>
+        <v>-1136652</v>
+      </c>
+      <c r="E65" s="11">
+        <f>IF(C65=0,"NEW",D65/C65)</f>
+        <v>-0.49514957703370793</v>
+      </c>
+      <c r="G65" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="H65" s="36">
+        <v>70425166</v>
+      </c>
+      <c r="I65" s="36">
+        <v>102812427</v>
+      </c>
+      <c r="J65" s="37">
+        <f>H65-I65</f>
+        <v>-32387261</v>
+      </c>
+      <c r="K65" s="38">
+        <f>IF(I65=0,"NEW",J65/I65)</f>
+        <v>-0.31501309661720173</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>103</v>
+      </c>
+      <c r="B66" s="1">
+        <v>1091690</v>
+      </c>
+      <c r="C66" s="1">
+        <v>1635003</v>
+      </c>
+      <c r="D66" s="10">
+        <f>B66-C66</f>
+        <v>-543313</v>
+      </c>
+      <c r="E66" s="11">
+        <f>IF(C66=0,"NEW",D66/C66)</f>
+        <v>-0.3323009193255303</v>
+      </c>
+      <c r="G66" s="39" t="s">
+        <v>119</v>
+      </c>
+      <c r="H66" s="40">
+        <v>68291120</v>
+      </c>
+      <c r="I66" s="40">
+        <v>75674760</v>
+      </c>
+      <c r="J66" s="41">
+        <f>H66-I66</f>
+        <v>-7383640</v>
+      </c>
+      <c r="K66" s="42">
+        <f>IF(I66=0,"NEW",J66/I66)</f>
+        <v>-9.7570709177009607E-2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>49</v>
+      </c>
+      <c r="B67" s="1">
+        <v>1084547</v>
+      </c>
+      <c r="C67" s="1">
+        <v>3738190</v>
+      </c>
+      <c r="D67" s="10">
+        <f>B67-C67</f>
+        <v>-2653643</v>
+      </c>
+      <c r="E67" s="11">
+        <f>IF(C67=0,"NEW",D67/C67)</f>
+        <v>-0.70987376243583122</v>
+      </c>
+      <c r="G67" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="H67" s="36">
+        <v>52081663</v>
+      </c>
+      <c r="I67" s="36">
+        <v>101571505</v>
+      </c>
+      <c r="J67" s="37">
+        <f>H67-I67</f>
+        <v>-49489842</v>
+      </c>
+      <c r="K67" s="38">
+        <f>IF(I67=0,"NEW",J67/I67)</f>
+        <v>-0.48724139708277436</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>51</v>
+      </c>
+      <c r="B68" s="1">
+        <v>1003658</v>
+      </c>
+      <c r="C68" s="1">
+        <v>1710177</v>
+      </c>
+      <c r="D68" s="10">
+        <f>B68-C68</f>
+        <v>-706519</v>
+      </c>
+      <c r="E68" s="11">
+        <f>IF(C68=0,"NEW",D68/C68)</f>
+        <v>-0.41312624365782019</v>
+      </c>
+      <c r="G68" s="39" t="s">
+        <v>59</v>
+      </c>
+      <c r="H68" s="40">
+        <v>50849324</v>
+      </c>
+      <c r="I68" s="40">
+        <v>96610083</v>
+      </c>
+      <c r="J68" s="41">
+        <f>H68-I68</f>
+        <v>-45760759</v>
+      </c>
+      <c r="K68" s="42">
+        <f>IF(I68=0,"NEW",J68/I68)</f>
+        <v>-0.47366442072097176</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>126</v>
+      </c>
+      <c r="B69" s="1">
+        <v>914003</v>
+      </c>
+      <c r="C69" s="1">
+        <v>1290126</v>
+      </c>
+      <c r="D69" s="10">
+        <f>B69-C69</f>
+        <v>-376123</v>
+      </c>
+      <c r="E69" s="11">
+        <f>IF(C69=0,"NEW",D69/C69)</f>
+        <v>-0.29153974107955349</v>
+      </c>
+      <c r="G69" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="H69" s="36">
+        <v>34292071</v>
+      </c>
+      <c r="I69" s="36">
+        <v>33423004</v>
+      </c>
+      <c r="J69" s="37">
+        <f>H69-I69</f>
+        <v>869067</v>
+      </c>
+      <c r="K69" s="38">
+        <f>IF(I69=0,"NEW",J69/I69)</f>
+        <v>2.6002061334762131E-2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>46</v>
+      </c>
+      <c r="B70" s="1">
+        <v>905868</v>
+      </c>
+      <c r="C70" s="1">
+        <v>1245685</v>
+      </c>
+      <c r="D70" s="10">
+        <f>B70-C70</f>
+        <v>-339817</v>
+      </c>
+      <c r="E70" s="11">
+        <f>IF(C70=0,"NEW",D70/C70)</f>
+        <v>-0.27279528933879754</v>
+      </c>
+      <c r="G70" s="39" t="s">
+        <v>81</v>
+      </c>
+      <c r="H70" s="40">
+        <v>30965147</v>
+      </c>
+      <c r="I70" s="40">
+        <v>23501652</v>
+      </c>
+      <c r="J70" s="41">
+        <f>H70-I70</f>
+        <v>7463495</v>
+      </c>
+      <c r="K70" s="42">
+        <f>IF(I70=0,"NEW",J70/I70)</f>
+        <v>0.31757320719411553</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>40</v>
+      </c>
+      <c r="B71" s="1">
+        <v>902209</v>
+      </c>
+      <c r="C71" s="1">
+        <v>988890</v>
+      </c>
+      <c r="D71" s="10">
+        <f>B71-C71</f>
+        <v>-86681</v>
+      </c>
+      <c r="E71" s="11">
+        <f>IF(C71=0,"NEW",D71/C71)</f>
+        <v>-8.7654845331634465E-2</v>
+      </c>
+      <c r="G71" s="35" t="s">
+        <v>96</v>
+      </c>
+      <c r="H71" s="36">
+        <v>21630069</v>
+      </c>
+      <c r="I71" s="36">
+        <v>29672513</v>
+      </c>
+      <c r="J71" s="37">
+        <f>H71-I71</f>
+        <v>-8042444</v>
+      </c>
+      <c r="K71" s="38">
+        <f>IF(I71=0,"NEW",J71/I71)</f>
+        <v>-0.27104020478481211</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
         <v>18</v>
       </c>
-      <c r="B23" s="1">
+      <c r="B72" s="1">
         <v>733247</v>
       </c>
-      <c r="C23" s="1">
+      <c r="C72" s="1">
         <v>1076602</v>
       </c>
-      <c r="D23" s="10">
-        <f t="shared" si="3"/>
+      <c r="D72" s="10">
+        <f>B72-C72</f>
         <v>-343355</v>
       </c>
-      <c r="E23" s="11">
-        <f t="shared" si="4"/>
+      <c r="E72" s="11">
+        <f>IF(C72=0,"NEW",D72/C72)</f>
         <v>-0.31892472798675836</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>19</v>
-      </c>
-      <c r="B24" s="1">
-        <v>0</v>
-      </c>
-      <c r="C24" s="1">
-        <v>41640</v>
-      </c>
-      <c r="D24" s="10">
-        <f t="shared" si="3"/>
-        <v>-41640</v>
-      </c>
-      <c r="E24" s="11">
-        <f t="shared" si="4"/>
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>20</v>
-      </c>
-      <c r="B25" s="1">
-        <v>70425166</v>
-      </c>
-      <c r="C25" s="1">
-        <v>102812427</v>
-      </c>
-      <c r="D25" s="10">
-        <f t="shared" si="3"/>
-        <v>-32387261</v>
-      </c>
-      <c r="E25" s="11">
-        <f t="shared" si="4"/>
-        <v>-0.31501309661720173</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>21</v>
-      </c>
-      <c r="B26" s="1">
-        <v>3613527</v>
-      </c>
-      <c r="C26" s="1">
-        <v>7795106</v>
-      </c>
-      <c r="D26" s="10">
-        <f t="shared" si="3"/>
-        <v>-4181579</v>
-      </c>
-      <c r="E26" s="11">
-        <f t="shared" si="4"/>
-        <v>-0.53643645128109863</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>22</v>
-      </c>
-      <c r="B27" s="1">
-        <v>422102</v>
-      </c>
-      <c r="C27" s="1">
-        <v>527689</v>
-      </c>
-      <c r="D27" s="10">
-        <f t="shared" si="3"/>
-        <v>-105587</v>
-      </c>
-      <c r="E27" s="11">
-        <f t="shared" si="4"/>
-        <v>-0.20009323673603202</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>23</v>
-      </c>
-      <c r="B28" s="1">
-        <v>334048</v>
-      </c>
-      <c r="C28" s="1">
-        <v>380204</v>
-      </c>
-      <c r="D28" s="10">
-        <f t="shared" si="3"/>
-        <v>-46156</v>
-      </c>
-      <c r="E28" s="11">
-        <f t="shared" si="4"/>
-        <v>-0.12139798634417313</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>24</v>
-      </c>
-      <c r="B29" s="1">
-        <v>65469</v>
-      </c>
-      <c r="C29" s="1">
-        <v>0</v>
-      </c>
-      <c r="D29" s="10">
-        <f t="shared" si="3"/>
-        <v>65469</v>
-      </c>
-      <c r="E29" s="11" t="str">
-        <f t="shared" si="4"/>
-        <v>NEW</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>25</v>
-      </c>
-      <c r="B30" s="1">
-        <v>36527</v>
-      </c>
-      <c r="C30" s="1">
-        <v>0</v>
-      </c>
-      <c r="D30" s="10">
-        <f t="shared" si="3"/>
-        <v>36527</v>
-      </c>
-      <c r="E30" s="11" t="str">
-        <f t="shared" si="4"/>
-        <v>NEW</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B31" s="1">
-        <v>81838</v>
-      </c>
-      <c r="C31" s="1">
-        <v>76354</v>
-      </c>
-      <c r="D31" s="10">
-        <f t="shared" si="3"/>
-        <v>5484</v>
-      </c>
-      <c r="E31" s="11">
-        <f t="shared" si="4"/>
-        <v>7.1823349136914891E-2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>27</v>
-      </c>
-      <c r="B32" s="1">
-        <v>10908743</v>
-      </c>
-      <c r="C32" s="1">
-        <v>18660355</v>
-      </c>
-      <c r="D32" s="10">
-        <f t="shared" si="3"/>
-        <v>-7751612</v>
-      </c>
-      <c r="E32" s="11">
-        <f t="shared" si="4"/>
-        <v>-0.41540538751808315</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
+      <c r="G72" s="39" t="s">
+        <v>115</v>
+      </c>
+      <c r="H72" s="40">
+        <v>15921847</v>
+      </c>
+      <c r="I72" s="40">
+        <v>25699820</v>
+      </c>
+      <c r="J72" s="41">
+        <f>H72-I72</f>
+        <v>-9777973</v>
+      </c>
+      <c r="K72" s="42">
+        <f>IF(I72=0,"NEW",J72/I72)</f>
+        <v>-0.38046854024658538</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>113</v>
+      </c>
+      <c r="B73" s="1">
+        <v>698561</v>
+      </c>
+      <c r="C73" s="1">
+        <v>1130404</v>
+      </c>
+      <c r="D73" s="10">
+        <f>B73-C73</f>
+        <v>-431843</v>
+      </c>
+      <c r="E73" s="11">
+        <f>IF(C73=0,"NEW",D73/C73)</f>
+        <v>-0.38202536438299933</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>104</v>
+      </c>
+      <c r="B74" s="1">
+        <v>682046</v>
+      </c>
+      <c r="C74" s="1">
+        <v>1421455</v>
+      </c>
+      <c r="D74" s="10">
+        <f>B74-C74</f>
+        <v>-739409</v>
+      </c>
+      <c r="E74" s="11">
+        <f>IF(C74=0,"NEW",D74/C74)</f>
+        <v>-0.52017756453774477</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>87</v>
+      </c>
+      <c r="B75" s="1">
+        <v>597794</v>
+      </c>
+      <c r="C75" s="1">
+        <v>1145273</v>
+      </c>
+      <c r="D75" s="10">
+        <f>B75-C75</f>
+        <v>-547479</v>
+      </c>
+      <c r="E75" s="11">
+        <f>IF(C75=0,"NEW",D75/C75)</f>
+        <v>-0.47803362167797547</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>92</v>
+      </c>
+      <c r="B76" s="1">
+        <v>580085</v>
+      </c>
+      <c r="C76" s="1">
+        <v>897670</v>
+      </c>
+      <c r="D76" s="10">
+        <f>B76-C76</f>
+        <v>-317585</v>
+      </c>
+      <c r="E76" s="11">
+        <f>IF(C76=0,"NEW",D76/C76)</f>
+        <v>-0.35378814040794504</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>120</v>
+      </c>
+      <c r="B77" s="1">
+        <v>576160</v>
+      </c>
+      <c r="C77" s="1">
+        <v>395859</v>
+      </c>
+      <c r="D77" s="10">
+        <f>B77-C77</f>
+        <v>180301</v>
+      </c>
+      <c r="E77" s="11">
+        <f>IF(C77=0,"NEW",D77/C77)</f>
+        <v>0.4554677296714234</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
         <v>28</v>
       </c>
-      <c r="B33" s="1">
+      <c r="B78" s="1">
         <v>540142</v>
       </c>
-      <c r="C33" s="1">
+      <c r="C78" s="1">
         <v>693272</v>
       </c>
-      <c r="D33" s="10">
-        <f t="shared" si="3"/>
+      <c r="D78" s="10">
+        <f>B78-C78</f>
         <v>-153130</v>
       </c>
-      <c r="E33" s="11">
-        <f t="shared" si="4"/>
+      <c r="E78" s="11">
+        <f>IF(C78=0,"NEW",D78/C78)</f>
         <v>-0.22088011631798196</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>29</v>
-      </c>
-      <c r="B34" s="1">
-        <v>1837345</v>
-      </c>
-      <c r="C34" s="1">
-        <v>5302363</v>
-      </c>
-      <c r="D34" s="10">
-        <f t="shared" si="3"/>
-        <v>-3465018</v>
-      </c>
-      <c r="E34" s="11">
-        <f t="shared" si="4"/>
-        <v>-0.65348562518258368</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>30</v>
-      </c>
-      <c r="B35" s="1">
-        <v>48873</v>
-      </c>
-      <c r="C35" s="1">
-        <v>17070</v>
-      </c>
-      <c r="D35" s="10">
-        <f t="shared" si="3"/>
-        <v>31803</v>
-      </c>
-      <c r="E35" s="11">
-        <f t="shared" si="4"/>
-        <v>1.8630931458699473</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>31</v>
-      </c>
-      <c r="B36" s="1">
-        <v>0</v>
-      </c>
-      <c r="C36" s="1">
-        <v>143790</v>
-      </c>
-      <c r="D36" s="10">
-        <f t="shared" si="3"/>
-        <v>-143790</v>
-      </c>
-      <c r="E36" s="11">
-        <f t="shared" si="4"/>
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>32</v>
-      </c>
-      <c r="B37" s="1">
-        <v>5458628</v>
-      </c>
-      <c r="C37" s="1">
-        <v>6987958</v>
-      </c>
-      <c r="D37" s="10">
-        <f t="shared" si="3"/>
-        <v>-1529330</v>
-      </c>
-      <c r="E37" s="11">
-        <f t="shared" si="4"/>
-        <v>-0.21885220260339286</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>33</v>
-      </c>
-      <c r="B38" s="1">
-        <v>3895474</v>
-      </c>
-      <c r="C38" s="1">
-        <v>6402257</v>
-      </c>
-      <c r="D38" s="10">
-        <f t="shared" si="3"/>
-        <v>-2506783</v>
-      </c>
-      <c r="E38" s="11">
-        <f t="shared" si="4"/>
-        <v>-0.39154676233709457</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>34</v>
-      </c>
-      <c r="B39" s="1">
-        <v>319160</v>
-      </c>
-      <c r="C39" s="1">
-        <v>697485</v>
-      </c>
-      <c r="D39" s="10">
-        <f t="shared" si="3"/>
-        <v>-378325</v>
-      </c>
-      <c r="E39" s="11">
-        <f t="shared" si="4"/>
-        <v>-0.5424130984895732</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>35</v>
-      </c>
-      <c r="B40" s="1">
-        <v>0</v>
-      </c>
-      <c r="C40" s="1">
-        <v>7737</v>
-      </c>
-      <c r="D40" s="10">
-        <f t="shared" si="3"/>
-        <v>-7737</v>
-      </c>
-      <c r="E40" s="11">
-        <f t="shared" si="4"/>
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>36</v>
-      </c>
-      <c r="B41" s="1">
-        <v>34292071</v>
-      </c>
-      <c r="C41" s="1">
-        <v>33423004</v>
-      </c>
-      <c r="D41" s="10">
-        <f t="shared" si="3"/>
-        <v>869067</v>
-      </c>
-      <c r="E41" s="11">
-        <f t="shared" si="4"/>
-        <v>2.6002061334762131E-2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>37</v>
-      </c>
-      <c r="B42" s="1">
-        <v>54417</v>
-      </c>
-      <c r="C42" s="1">
-        <v>30835</v>
-      </c>
-      <c r="D42" s="10">
-        <f t="shared" si="3"/>
-        <v>23582</v>
-      </c>
-      <c r="E42" s="11">
-        <f t="shared" si="4"/>
-        <v>0.76478028214691096</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>38</v>
-      </c>
-      <c r="B43" s="1">
-        <v>6714270</v>
-      </c>
-      <c r="C43" s="1">
-        <v>12390236</v>
-      </c>
-      <c r="D43" s="10">
-        <f t="shared" si="3"/>
-        <v>-5675966</v>
-      </c>
-      <c r="E43" s="11">
-        <f t="shared" si="4"/>
-        <v>-0.45809991028419472</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>39</v>
-      </c>
-      <c r="B44" s="1">
-        <v>4170090</v>
-      </c>
-      <c r="C44" s="1">
-        <v>4467702</v>
-      </c>
-      <c r="D44" s="10">
-        <f t="shared" si="3"/>
-        <v>-297612</v>
-      </c>
-      <c r="E44" s="11">
-        <f t="shared" si="4"/>
-        <v>-6.6614111684261845E-2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>40</v>
-      </c>
-      <c r="B45" s="1">
-        <v>902209</v>
-      </c>
-      <c r="C45" s="1">
-        <v>988890</v>
-      </c>
-      <c r="D45" s="10">
-        <f t="shared" si="3"/>
-        <v>-86681</v>
-      </c>
-      <c r="E45" s="11">
-        <f t="shared" si="4"/>
-        <v>-8.7654845331634465E-2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>41</v>
-      </c>
-      <c r="B46" s="1">
-        <v>0</v>
-      </c>
-      <c r="C46" s="1">
-        <v>34450</v>
-      </c>
-      <c r="D46" s="10">
-        <f t="shared" si="3"/>
-        <v>-34450</v>
-      </c>
-      <c r="E46" s="11">
-        <f t="shared" si="4"/>
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>42</v>
-      </c>
-      <c r="B47" s="1">
-        <v>182646</v>
-      </c>
-      <c r="C47" s="1">
-        <v>86307</v>
-      </c>
-      <c r="D47" s="10">
-        <f t="shared" si="3"/>
-        <v>96339</v>
-      </c>
-      <c r="E47" s="11">
-        <f t="shared" si="4"/>
-        <v>1.1162362264937955</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>43</v>
-      </c>
-      <c r="B48" s="1">
-        <v>2125328</v>
-      </c>
-      <c r="C48" s="1">
-        <v>3743552</v>
-      </c>
-      <c r="D48" s="10">
-        <f t="shared" si="3"/>
-        <v>-1618224</v>
-      </c>
-      <c r="E48" s="11">
-        <f t="shared" si="4"/>
-        <v>-0.43226967329424032</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>44</v>
-      </c>
-      <c r="B49" s="1">
-        <v>56385</v>
-      </c>
-      <c r="C49" s="1">
-        <v>0</v>
-      </c>
-      <c r="D49" s="10">
-        <f t="shared" si="3"/>
-        <v>56385</v>
-      </c>
-      <c r="E49" s="11" t="str">
-        <f t="shared" si="4"/>
-        <v>NEW</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
-        <v>45</v>
-      </c>
-      <c r="B50" s="1">
-        <v>14655</v>
-      </c>
-      <c r="C50" s="1">
-        <v>64583</v>
-      </c>
-      <c r="D50" s="10">
-        <f t="shared" si="3"/>
-        <v>-49928</v>
-      </c>
-      <c r="E50" s="11">
-        <f t="shared" si="4"/>
-        <v>-0.77308269978167632</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
-        <v>46</v>
-      </c>
-      <c r="B51" s="1">
-        <v>905868</v>
-      </c>
-      <c r="C51" s="1">
-        <v>1245685</v>
-      </c>
-      <c r="D51" s="10">
-        <f t="shared" si="3"/>
-        <v>-339817</v>
-      </c>
-      <c r="E51" s="11">
-        <f t="shared" si="4"/>
-        <v>-0.27279528933879754</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
-        <v>49</v>
-      </c>
-      <c r="B52" s="1">
-        <v>1084547</v>
-      </c>
-      <c r="C52" s="1">
-        <v>3738190</v>
-      </c>
-      <c r="D52" s="10">
-        <f t="shared" si="3"/>
-        <v>-2653643</v>
-      </c>
-      <c r="E52" s="11">
-        <f t="shared" si="4"/>
-        <v>-0.70987376243583122</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
-        <v>47</v>
-      </c>
-      <c r="B53" s="1">
-        <v>1786170</v>
-      </c>
-      <c r="C53" s="1">
-        <v>2284321</v>
-      </c>
-      <c r="D53" s="10">
-        <f t="shared" si="3"/>
-        <v>-498151</v>
-      </c>
-      <c r="E53" s="11">
-        <f t="shared" si="4"/>
-        <v>-0.21807399222788743</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
-        <v>48</v>
-      </c>
-      <c r="B54" s="1">
-        <v>450114</v>
-      </c>
-      <c r="C54" s="1">
-        <v>592724</v>
-      </c>
-      <c r="D54" s="10">
-        <f t="shared" si="3"/>
-        <v>-142610</v>
-      </c>
-      <c r="E54" s="11">
-        <f t="shared" si="4"/>
-        <v>-0.24060102172343284</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
-        <v>50</v>
-      </c>
-      <c r="B55" s="1">
-        <v>22973</v>
-      </c>
-      <c r="C55" s="1">
-        <v>11776</v>
-      </c>
-      <c r="D55" s="10">
-        <f t="shared" si="3"/>
-        <v>11197</v>
-      </c>
-      <c r="E55" s="11">
-        <f t="shared" si="4"/>
-        <v>0.95083220108695654</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
-        <v>51</v>
-      </c>
-      <c r="B56" s="1">
-        <v>1003658</v>
-      </c>
-      <c r="C56" s="1">
-        <v>1710177</v>
-      </c>
-      <c r="D56" s="10">
-        <f t="shared" si="3"/>
-        <v>-706519</v>
-      </c>
-      <c r="E56" s="11">
-        <f t="shared" si="4"/>
-        <v>-0.41312624365782019</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
-        <v>52</v>
-      </c>
-      <c r="B57" s="1">
-        <v>248075</v>
-      </c>
-      <c r="C57" s="1">
-        <v>2064191</v>
-      </c>
-      <c r="D57" s="10">
-        <f t="shared" si="3"/>
-        <v>-1816116</v>
-      </c>
-      <c r="E57" s="11">
-        <f t="shared" si="4"/>
-        <v>-0.87981974536271113</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
-        <v>53</v>
-      </c>
-      <c r="B58" s="1">
-        <v>12608</v>
-      </c>
-      <c r="C58" s="1">
-        <v>6780</v>
-      </c>
-      <c r="D58" s="10">
-        <f t="shared" si="3"/>
-        <v>5828</v>
-      </c>
-      <c r="E58" s="11">
-        <f t="shared" si="4"/>
-        <v>0.85958702064896753</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
-        <v>54</v>
-      </c>
-      <c r="B59" s="1">
-        <v>2044602</v>
-      </c>
-      <c r="C59" s="1">
-        <v>2802152</v>
-      </c>
-      <c r="D59" s="10">
-        <f t="shared" si="3"/>
-        <v>-757550</v>
-      </c>
-      <c r="E59" s="11">
-        <f t="shared" si="4"/>
-        <v>-0.27034579137748416</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
-        <v>55</v>
-      </c>
-      <c r="B60" s="1">
-        <v>96600</v>
-      </c>
-      <c r="C60" s="1">
-        <v>232960</v>
-      </c>
-      <c r="D60" s="10">
-        <f t="shared" si="3"/>
-        <v>-136360</v>
-      </c>
-      <c r="E60" s="11">
-        <f t="shared" si="4"/>
-        <v>-0.58533653846153844</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
-        <v>56</v>
-      </c>
-      <c r="B61" s="1">
-        <v>102807</v>
-      </c>
-      <c r="C61" s="1">
-        <v>260354</v>
-      </c>
-      <c r="D61" s="10">
-        <f t="shared" si="3"/>
-        <v>-157547</v>
-      </c>
-      <c r="E61" s="11">
-        <f t="shared" si="4"/>
-        <v>-0.60512609754411306</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
-        <v>57</v>
-      </c>
-      <c r="B62" s="1">
-        <v>52081663</v>
-      </c>
-      <c r="C62" s="1">
-        <v>101571505</v>
-      </c>
-      <c r="D62" s="10">
-        <f t="shared" si="3"/>
-        <v>-49489842</v>
-      </c>
-      <c r="E62" s="11">
-        <f t="shared" si="4"/>
-        <v>-0.48724139708277436</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
-        <v>58</v>
-      </c>
-      <c r="B63" s="1">
-        <v>5062153</v>
-      </c>
-      <c r="C63" s="1">
-        <v>7788444</v>
-      </c>
-      <c r="D63" s="10">
-        <f t="shared" si="3"/>
-        <v>-2726291</v>
-      </c>
-      <c r="E63" s="11">
-        <f t="shared" si="4"/>
-        <v>-0.35004308947974716</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
-        <v>59</v>
-      </c>
-      <c r="B64" s="1">
-        <v>50849324</v>
-      </c>
-      <c r="C64" s="1">
-        <v>96610083</v>
-      </c>
-      <c r="D64" s="10">
-        <f t="shared" si="3"/>
-        <v>-45760759</v>
-      </c>
-      <c r="E64" s="11">
-        <f t="shared" si="4"/>
-        <v>-0.47366442072097176</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A65" t="s">
-        <v>60</v>
-      </c>
-      <c r="B65" s="1">
-        <v>2384085</v>
-      </c>
-      <c r="C65" s="1">
-        <v>9798667</v>
-      </c>
-      <c r="D65" s="10">
-        <f t="shared" si="3"/>
-        <v>-7414582</v>
-      </c>
-      <c r="E65" s="11">
-        <f t="shared" si="4"/>
-        <v>-0.75669292568060531</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A66" t="s">
-        <v>61</v>
-      </c>
-      <c r="B66" s="1">
-        <v>0</v>
-      </c>
-      <c r="C66" s="1">
-        <v>9251</v>
-      </c>
-      <c r="D66" s="10">
-        <f t="shared" si="3"/>
-        <v>-9251</v>
-      </c>
-      <c r="E66" s="11">
-        <f t="shared" si="4"/>
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
-        <v>62</v>
-      </c>
-      <c r="B67" s="1">
-        <v>228869</v>
-      </c>
-      <c r="C67" s="1">
-        <v>273521</v>
-      </c>
-      <c r="D67" s="10">
-        <f t="shared" si="3"/>
-        <v>-44652</v>
-      </c>
-      <c r="E67" s="11">
-        <f t="shared" si="4"/>
-        <v>-0.16324889130999082</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A68" t="s">
-        <v>63</v>
-      </c>
-      <c r="B68" s="1">
-        <v>93292</v>
-      </c>
-      <c r="C68" s="1">
-        <v>277910</v>
-      </c>
-      <c r="D68" s="10">
-        <f t="shared" si="3"/>
-        <v>-184618</v>
-      </c>
-      <c r="E68" s="11">
-        <f t="shared" si="4"/>
-        <v>-0.66430858911158286</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A69" t="s">
-        <v>64</v>
-      </c>
-      <c r="B69" s="1">
-        <v>0</v>
-      </c>
-      <c r="C69" s="1">
-        <v>3037</v>
-      </c>
-      <c r="D69" s="10">
-        <f t="shared" si="3"/>
-        <v>-3037</v>
-      </c>
-      <c r="E69" s="11">
-        <f t="shared" si="4"/>
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A70" t="s">
-        <v>65</v>
-      </c>
-      <c r="B70" s="1">
-        <v>55485</v>
-      </c>
-      <c r="C70" s="1">
-        <v>88965</v>
-      </c>
-      <c r="D70" s="10">
-        <f t="shared" si="3"/>
-        <v>-33480</v>
-      </c>
-      <c r="E70" s="11">
-        <f t="shared" si="4"/>
-        <v>-0.37632776934749623</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A71" t="s">
-        <v>66</v>
-      </c>
-      <c r="B71" s="1">
-        <v>18300</v>
-      </c>
-      <c r="C71" s="1">
-        <v>29625</v>
-      </c>
-      <c r="D71" s="10">
-        <f t="shared" si="3"/>
-        <v>-11325</v>
-      </c>
-      <c r="E71" s="11">
-        <f t="shared" si="4"/>
-        <v>-0.38227848101265821</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A72" t="s">
-        <v>67</v>
-      </c>
-      <c r="B72" s="1">
-        <v>1615940</v>
-      </c>
-      <c r="C72" s="1">
-        <v>2232330</v>
-      </c>
-      <c r="D72" s="10">
-        <f t="shared" si="3"/>
-        <v>-616390</v>
-      </c>
-      <c r="E72" s="11">
-        <f t="shared" si="4"/>
-        <v>-0.27611957013523986</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A73" t="s">
-        <v>68</v>
-      </c>
-      <c r="B73" s="1">
-        <v>1158921</v>
-      </c>
-      <c r="C73" s="1">
-        <v>2295573</v>
-      </c>
-      <c r="D73" s="10">
-        <f t="shared" si="3"/>
-        <v>-1136652</v>
-      </c>
-      <c r="E73" s="11">
-        <f t="shared" si="4"/>
-        <v>-0.49514957703370793</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A74" t="s">
-        <v>69</v>
-      </c>
-      <c r="B74" s="1">
-        <v>90410</v>
-      </c>
-      <c r="C74" s="1">
-        <v>222096</v>
-      </c>
-      <c r="D74" s="10">
-        <f t="shared" si="3"/>
-        <v>-131686</v>
-      </c>
-      <c r="E74" s="11">
-        <f t="shared" si="4"/>
-        <v>-0.59292378070744178</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A75" t="s">
-        <v>70</v>
-      </c>
-      <c r="B75" s="1">
-        <v>1985216</v>
-      </c>
-      <c r="C75" s="1">
-        <v>3582648</v>
-      </c>
-      <c r="D75" s="10">
-        <f t="shared" si="3"/>
-        <v>-1597432</v>
-      </c>
-      <c r="E75" s="11">
-        <f t="shared" si="4"/>
-        <v>-0.44588025393507819</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A76" t="s">
-        <v>71</v>
-      </c>
-      <c r="B76" s="1">
-        <v>9098</v>
-      </c>
-      <c r="C76" s="1">
-        <v>0</v>
-      </c>
-      <c r="D76" s="10">
-        <f t="shared" si="3"/>
-        <v>9098</v>
-      </c>
-      <c r="E76" s="11" t="str">
-        <f t="shared" si="4"/>
-        <v>NEW</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A77" t="s">
-        <v>72</v>
-      </c>
-      <c r="B77" s="1">
-        <v>2585959</v>
-      </c>
-      <c r="C77" s="1">
-        <v>4075159</v>
-      </c>
-      <c r="D77" s="10">
-        <f t="shared" si="3"/>
-        <v>-1489200</v>
-      </c>
-      <c r="E77" s="11">
-        <f t="shared" si="4"/>
-        <v>-0.36543359412479365</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A78" t="s">
-        <v>73</v>
-      </c>
-      <c r="B78" s="1">
-        <v>2576157</v>
-      </c>
-      <c r="C78" s="1">
-        <v>3406976</v>
-      </c>
-      <c r="D78" s="10">
-        <f t="shared" si="3"/>
-        <v>-830819</v>
-      </c>
-      <c r="E78" s="11">
-        <f t="shared" si="4"/>
-        <v>-0.24385818978472404</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>74</v>
+        <v>108</v>
       </c>
       <c r="B79" s="1">
-        <v>14348603</v>
+        <v>526282</v>
       </c>
       <c r="C79" s="1">
-        <v>27439305</v>
+        <v>395395</v>
       </c>
       <c r="D79" s="10">
-        <f t="shared" si="3"/>
-        <v>-13090702</v>
+        <f>B79-C79</f>
+        <v>130887</v>
       </c>
       <c r="E79" s="11">
-        <f t="shared" si="4"/>
-        <v>-0.4770784828551598</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+        <f>IF(C79=0,"NEW",D79/C79)</f>
+        <v>0.33102846520568041</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="B80" s="1">
-        <v>439724</v>
+        <v>506600</v>
       </c>
       <c r="C80" s="1">
-        <v>444958</v>
+        <v>1081764</v>
       </c>
       <c r="D80" s="10">
-        <f t="shared" si="3"/>
-        <v>-5234</v>
+        <f>B80-C80</f>
+        <v>-575164</v>
       </c>
       <c r="E80" s="11">
-        <f t="shared" si="4"/>
-        <v>-1.176290795985239E-2</v>
+        <f>IF(C80=0,"NEW",D80/C80)</f>
+        <v>-0.5316908309021191</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>76</v>
+        <v>138</v>
       </c>
       <c r="B81" s="1">
-        <v>72746897</v>
+        <v>450663</v>
       </c>
       <c r="C81" s="1">
-        <v>72882617</v>
+        <v>449503</v>
       </c>
       <c r="D81" s="10">
-        <f t="shared" si="3"/>
-        <v>-135720</v>
+        <f>B81-C81</f>
+        <v>1160</v>
       </c>
       <c r="E81" s="11">
-        <f t="shared" si="4"/>
-        <v>-1.862172429949929E-3</v>
+        <f>IF(C81=0,"NEW",D81/C81)</f>
+        <v>2.5806279379670437E-3</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>77</v>
+        <v>48</v>
       </c>
       <c r="B82" s="1">
-        <v>221566</v>
+        <v>450114</v>
       </c>
       <c r="C82" s="1">
-        <v>261558</v>
+        <v>592724</v>
       </c>
       <c r="D82" s="10">
-        <f t="shared" si="3"/>
-        <v>-39992</v>
+        <f>B82-C82</f>
+        <v>-142610</v>
       </c>
       <c r="E82" s="11">
-        <f t="shared" si="4"/>
-        <v>-0.15289916576820436</v>
+        <f>IF(C82=0,"NEW",D82/C82)</f>
+        <v>-0.24060102172343284</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B83" s="1">
-        <v>60690</v>
+        <v>439724</v>
       </c>
       <c r="C83" s="1">
-        <v>65205</v>
+        <v>444958</v>
       </c>
       <c r="D83" s="10">
-        <f t="shared" si="3"/>
-        <v>-4515</v>
+        <f>B83-C83</f>
+        <v>-5234</v>
       </c>
       <c r="E83" s="11">
-        <f t="shared" si="4"/>
-        <v>-6.9243156199677941E-2</v>
+        <f>IF(C83=0,"NEW",D83/C83)</f>
+        <v>-1.176290795985239E-2</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>79</v>
+        <v>22</v>
       </c>
       <c r="B84" s="1">
-        <v>8235</v>
+        <v>422102</v>
       </c>
       <c r="C84" s="1">
-        <v>12046</v>
+        <v>527689</v>
       </c>
       <c r="D84" s="10">
-        <f t="shared" si="3"/>
-        <v>-3811</v>
+        <f>B84-C84</f>
+        <v>-105587</v>
       </c>
       <c r="E84" s="11">
-        <f t="shared" si="4"/>
-        <v>-0.3163705794454591</v>
+        <f>IF(C84=0,"NEW",D84/C84)</f>
+        <v>-0.20009323673603202</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>80</v>
+        <v>107</v>
       </c>
       <c r="B85" s="1">
-        <v>2333826</v>
+        <v>362631</v>
       </c>
       <c r="C85" s="1">
-        <v>2826572</v>
+        <v>1915198</v>
       </c>
       <c r="D85" s="10">
-        <f t="shared" ref="D85:D144" si="5">B85-C85</f>
-        <v>-492746</v>
+        <f>B85-C85</f>
+        <v>-1552567</v>
       </c>
       <c r="E85" s="11">
-        <f t="shared" ref="E85:E144" si="6">IF(C85=0,"NEW",D85/C85)</f>
-        <v>-0.17432635715630099</v>
+        <f>IF(C85=0,"NEW",D85/C85)</f>
+        <v>-0.8106561305932859</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>81</v>
+        <v>123</v>
       </c>
       <c r="B86" s="1">
-        <v>30965147</v>
+        <v>352259</v>
       </c>
       <c r="C86" s="1">
-        <v>23501652</v>
+        <v>479898</v>
       </c>
       <c r="D86" s="10">
-        <f t="shared" si="5"/>
-        <v>7463495</v>
+        <f>B86-C86</f>
+        <v>-127639</v>
       </c>
       <c r="E86" s="11">
-        <f t="shared" si="6"/>
-        <v>0.31757320719411553</v>
+        <f>IF(C86=0,"NEW",D86/C86)</f>
+        <v>-0.26597110219254927</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>82</v>
+        <v>23</v>
       </c>
       <c r="B87" s="1">
-        <v>506600</v>
+        <v>334048</v>
       </c>
       <c r="C87" s="1">
-        <v>1081764</v>
+        <v>380204</v>
       </c>
       <c r="D87" s="10">
-        <f t="shared" si="5"/>
-        <v>-575164</v>
+        <f>B87-C87</f>
+        <v>-46156</v>
       </c>
       <c r="E87" s="11">
-        <f t="shared" si="6"/>
-        <v>-0.5316908309021191</v>
+        <f>IF(C87=0,"NEW",D87/C87)</f>
+        <v>-0.12139798634417313</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>83</v>
+        <v>34</v>
       </c>
       <c r="B88" s="1">
-        <v>2745172</v>
+        <v>319160</v>
       </c>
       <c r="C88" s="1">
-        <v>4125306</v>
+        <v>697485</v>
       </c>
       <c r="D88" s="10">
-        <f t="shared" si="5"/>
-        <v>-1380134</v>
+        <f>B88-C88</f>
+        <v>-378325</v>
       </c>
       <c r="E88" s="11">
-        <f t="shared" si="6"/>
-        <v>-0.33455312163509809</v>
+        <f>IF(C88=0,"NEW",D88/C88)</f>
+        <v>-0.5424130984895732</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="B89" s="1">
-        <v>242650</v>
+        <v>271136</v>
       </c>
       <c r="C89" s="1">
-        <v>10570</v>
+        <v>350114</v>
       </c>
       <c r="D89" s="10">
-        <f t="shared" si="5"/>
-        <v>232080</v>
+        <f>B89-C89</f>
+        <v>-78978</v>
       </c>
       <c r="E89" s="11">
-        <f t="shared" si="6"/>
-        <v>21.956480605487229</v>
+        <f>IF(C89=0,"NEW",D89/C89)</f>
+        <v>-0.22557795460907018</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>85</v>
+        <v>52</v>
       </c>
       <c r="B90" s="1">
-        <v>7800</v>
+        <v>248075</v>
       </c>
       <c r="C90" s="1">
-        <v>19210</v>
+        <v>2064191</v>
       </c>
       <c r="D90" s="10">
-        <f t="shared" si="5"/>
-        <v>-11410</v>
+        <f>B90-C90</f>
+        <v>-1816116</v>
       </c>
       <c r="E90" s="11">
-        <f t="shared" si="6"/>
-        <v>-0.59396147839666835</v>
+        <f>IF(C90=0,"NEW",D90/C90)</f>
+        <v>-0.87981974536271113</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B91" s="1">
-        <v>70292</v>
+        <v>242650</v>
       </c>
       <c r="C91" s="1">
-        <v>105290</v>
+        <v>10570</v>
       </c>
       <c r="D91" s="10">
-        <f t="shared" si="5"/>
-        <v>-34998</v>
+        <f>B91-C91</f>
+        <v>232080</v>
       </c>
       <c r="E91" s="11">
-        <f t="shared" si="6"/>
-        <v>-0.33239623895906545</v>
+        <f>IF(C91=0,"NEW",D91/C91)</f>
+        <v>21.956480605487229</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>87</v>
+        <v>62</v>
       </c>
       <c r="B92" s="1">
-        <v>597794</v>
+        <v>228869</v>
       </c>
       <c r="C92" s="1">
-        <v>1145273</v>
+        <v>273521</v>
       </c>
       <c r="D92" s="10">
-        <f t="shared" si="5"/>
-        <v>-547479</v>
+        <f>B92-C92</f>
+        <v>-44652</v>
       </c>
       <c r="E92" s="11">
-        <f t="shared" si="6"/>
-        <v>-0.47803362167797547</v>
+        <f>IF(C92=0,"NEW",D92/C92)</f>
+        <v>-0.16324889130999082</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B93" s="1">
-        <v>23793</v>
+        <v>226294</v>
       </c>
       <c r="C93" s="1">
-        <v>0</v>
+        <v>569363</v>
       </c>
       <c r="D93" s="10">
-        <f t="shared" si="5"/>
-        <v>23793</v>
-      </c>
-      <c r="E93" s="11" t="str">
-        <f t="shared" si="6"/>
-        <v>NEW</v>
+        <f>B93-C93</f>
+        <v>-343069</v>
+      </c>
+      <c r="E93" s="11">
+        <f>IF(C93=0,"NEW",D93/C93)</f>
+        <v>-0.60254881332295918</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="B94" s="1">
-        <v>226294</v>
+        <v>221566</v>
       </c>
       <c r="C94" s="1">
-        <v>569363</v>
+        <v>261558</v>
       </c>
       <c r="D94" s="10">
-        <f t="shared" si="5"/>
-        <v>-343069</v>
+        <f>B94-C94</f>
+        <v>-39992</v>
       </c>
       <c r="E94" s="11">
-        <f t="shared" si="6"/>
-        <v>-0.60254881332295918</v>
+        <f>IF(C94=0,"NEW",D94/C94)</f>
+        <v>-0.15289916576820436</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>90</v>
+        <v>111</v>
       </c>
       <c r="B95" s="1">
-        <v>8684806</v>
+        <v>196000</v>
       </c>
       <c r="C95" s="1">
-        <v>10043085</v>
+        <v>91056</v>
       </c>
       <c r="D95" s="10">
-        <f t="shared" si="5"/>
-        <v>-1358279</v>
+        <f>B95-C95</f>
+        <v>104944</v>
       </c>
       <c r="E95" s="11">
-        <f t="shared" si="6"/>
-        <v>-0.13524519607272067</v>
+        <f>IF(C95=0,"NEW",D95/C95)</f>
+        <v>1.1525215252152521</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>91</v>
+        <v>42</v>
       </c>
       <c r="B96" s="1">
-        <v>271136</v>
+        <v>182646</v>
       </c>
       <c r="C96" s="1">
-        <v>350114</v>
+        <v>86307</v>
       </c>
       <c r="D96" s="10">
-        <f t="shared" si="5"/>
-        <v>-78978</v>
+        <f>B96-C96</f>
+        <v>96339</v>
       </c>
       <c r="E96" s="11">
-        <f t="shared" si="6"/>
-        <v>-0.22557795460907018</v>
+        <f>IF(C96=0,"NEW",D96/C96)</f>
+        <v>1.1162362264937955</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>92</v>
+        <v>56</v>
       </c>
       <c r="B97" s="1">
-        <v>580085</v>
+        <v>102807</v>
       </c>
       <c r="C97" s="1">
-        <v>897670</v>
+        <v>260354</v>
       </c>
       <c r="D97" s="10">
-        <f t="shared" si="5"/>
-        <v>-317585</v>
+        <f>B97-C97</f>
+        <v>-157547</v>
       </c>
       <c r="E97" s="11">
-        <f t="shared" si="6"/>
-        <v>-0.35378814040794504</v>
+        <f>IF(C97=0,"NEW",D97/C97)</f>
+        <v>-0.60512609754411306</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>93</v>
+        <v>109</v>
       </c>
       <c r="B98" s="1">
-        <v>13543865</v>
+        <v>99385</v>
       </c>
       <c r="C98" s="1">
-        <v>19870728</v>
+        <v>0</v>
       </c>
       <c r="D98" s="10">
-        <f t="shared" si="5"/>
-        <v>-6326863</v>
-      </c>
-      <c r="E98" s="11">
-        <f t="shared" si="6"/>
-        <v>-0.31840116778811528</v>
+        <f>B98-C98</f>
+        <v>99385</v>
+      </c>
+      <c r="E98" s="11" t="str">
+        <f>IF(C98=0,"NEW",D98/C98)</f>
+        <v>NEW</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>94</v>
+        <v>55</v>
       </c>
       <c r="B99" s="1">
-        <v>5746</v>
+        <v>96600</v>
       </c>
       <c r="C99" s="1">
-        <v>132515</v>
+        <v>232960</v>
       </c>
       <c r="D99" s="10">
-        <f t="shared" si="5"/>
-        <v>-126769</v>
+        <f>B99-C99</f>
+        <v>-136360</v>
       </c>
       <c r="E99" s="11">
-        <f t="shared" si="6"/>
-        <v>-0.95663887107119949</v>
+        <f>IF(C99=0,"NEW",D99/C99)</f>
+        <v>-0.58533653846153844</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>95</v>
+        <v>63</v>
       </c>
       <c r="B100" s="1">
-        <v>0</v>
+        <v>93292</v>
       </c>
       <c r="C100" s="1">
-        <v>36935</v>
+        <v>277910</v>
       </c>
       <c r="D100" s="10">
-        <f t="shared" si="5"/>
-        <v>-36935</v>
+        <f>B100-C100</f>
+        <v>-184618</v>
       </c>
       <c r="E100" s="11">
-        <f t="shared" si="6"/>
-        <v>-1</v>
+        <f>IF(C100=0,"NEW",D100/C100)</f>
+        <v>-0.66430858911158286</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>96</v>
+        <v>69</v>
       </c>
       <c r="B101" s="1">
-        <v>21630069</v>
+        <v>90410</v>
       </c>
       <c r="C101" s="1">
-        <v>29672513</v>
+        <v>222096</v>
       </c>
       <c r="D101" s="10">
-        <f t="shared" si="5"/>
-        <v>-8042444</v>
+        <f>B101-C101</f>
+        <v>-131686</v>
       </c>
       <c r="E101" s="11">
-        <f t="shared" si="6"/>
-        <v>-0.27104020478481211</v>
+        <f>IF(C101=0,"NEW",D101/C101)</f>
+        <v>-0.59292378070744178</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>97</v>
+        <v>122</v>
       </c>
       <c r="B102" s="1">
-        <v>0</v>
+        <v>88919</v>
       </c>
       <c r="C102" s="1">
-        <v>35986</v>
+        <v>81554</v>
       </c>
       <c r="D102" s="10">
-        <f t="shared" si="5"/>
-        <v>-35986</v>
+        <f>B102-C102</f>
+        <v>7365</v>
       </c>
       <c r="E102" s="11">
-        <f t="shared" si="6"/>
-        <v>-1</v>
+        <f>IF(C102=0,"NEW",D102/C102)</f>
+        <v>9.030826201044706E-2</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>98</v>
+        <v>26</v>
       </c>
       <c r="B103" s="1">
-        <v>7740</v>
+        <v>81838</v>
       </c>
       <c r="C103" s="1">
-        <v>0</v>
+        <v>76354</v>
       </c>
       <c r="D103" s="10">
-        <f t="shared" si="5"/>
-        <v>7740</v>
-      </c>
-      <c r="E103" s="11" t="str">
-        <f t="shared" si="6"/>
-        <v>NEW</v>
+        <f>B103-C103</f>
+        <v>5484</v>
+      </c>
+      <c r="E103" s="11">
+        <f>IF(C103=0,"NEW",D103/C103)</f>
+        <v>7.1823349136914891E-2</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="B104" s="1">
-        <v>0</v>
+        <v>70292</v>
       </c>
       <c r="C104" s="1">
-        <v>1075001</v>
+        <v>105290</v>
       </c>
       <c r="D104" s="10">
-        <f t="shared" si="5"/>
-        <v>-1075001</v>
+        <f>B104-C104</f>
+        <v>-34998</v>
       </c>
       <c r="E104" s="11">
-        <f t="shared" si="6"/>
-        <v>-1</v>
+        <f>IF(C104=0,"NEW",D104/C104)</f>
+        <v>-0.33239623895906545</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>100</v>
+        <v>135</v>
       </c>
       <c r="B105" s="1">
-        <v>1262975</v>
+        <v>68387</v>
       </c>
       <c r="C105" s="1">
-        <v>2428500</v>
+        <v>352823</v>
       </c>
       <c r="D105" s="10">
-        <f t="shared" si="5"/>
-        <v>-1165525</v>
+        <f>B105-C105</f>
+        <v>-284436</v>
       </c>
       <c r="E105" s="11">
-        <f t="shared" si="6"/>
-        <v>-0.4799361745933704</v>
+        <f>IF(C105=0,"NEW",D105/C105)</f>
+        <v>-0.80617193323564507</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>101</v>
+        <v>24</v>
       </c>
       <c r="B106" s="1">
+        <v>65469</v>
+      </c>
+      <c r="C106" s="1">
         <v>0</v>
       </c>
-      <c r="C106" s="1">
-        <v>28041</v>
-      </c>
       <c r="D106" s="10">
-        <f t="shared" si="5"/>
-        <v>-28041</v>
-      </c>
-      <c r="E106" s="11">
-        <f t="shared" si="6"/>
-        <v>-1</v>
+        <f>B106-C106</f>
+        <v>65469</v>
+      </c>
+      <c r="E106" s="11" t="str">
+        <f>IF(C106=0,"NEW",D106/C106)</f>
+        <v>NEW</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>102</v>
+        <v>78</v>
       </c>
       <c r="B107" s="1">
-        <v>3632068</v>
+        <v>60690</v>
       </c>
       <c r="C107" s="1">
-        <v>6565377</v>
+        <v>65205</v>
       </c>
       <c r="D107" s="10">
-        <f t="shared" si="5"/>
-        <v>-2933309</v>
+        <f>B107-C107</f>
+        <v>-4515</v>
       </c>
       <c r="E107" s="11">
-        <f t="shared" si="6"/>
-        <v>-0.44678454870146833</v>
+        <f>IF(C107=0,"NEW",D107/C107)</f>
+        <v>-6.9243156199677941E-2</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>103</v>
+        <v>44</v>
       </c>
       <c r="B108" s="1">
-        <v>1091690</v>
+        <v>56385</v>
       </c>
       <c r="C108" s="1">
-        <v>1635003</v>
+        <v>0</v>
       </c>
       <c r="D108" s="10">
-        <f t="shared" si="5"/>
-        <v>-543313</v>
-      </c>
-      <c r="E108" s="11">
-        <f t="shared" si="6"/>
-        <v>-0.3323009193255303</v>
+        <f>B108-C108</f>
+        <v>56385</v>
+      </c>
+      <c r="E108" s="11" t="str">
+        <f>IF(C108=0,"NEW",D108/C108)</f>
+        <v>NEW</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>104</v>
+        <v>65</v>
       </c>
       <c r="B109" s="1">
-        <v>682046</v>
+        <v>55485</v>
       </c>
       <c r="C109" s="1">
-        <v>1421455</v>
+        <v>88965</v>
       </c>
       <c r="D109" s="10">
-        <f t="shared" si="5"/>
-        <v>-739409</v>
+        <f>B109-C109</f>
+        <v>-33480</v>
       </c>
       <c r="E109" s="11">
-        <f t="shared" si="6"/>
-        <v>-0.52017756453774477</v>
+        <f>IF(C109=0,"NEW",D109/C109)</f>
+        <v>-0.37632776934749623</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>105</v>
+        <v>37</v>
       </c>
       <c r="B110" s="1">
-        <v>2057002</v>
+        <v>54417</v>
       </c>
       <c r="C110" s="1">
-        <v>369609</v>
+        <v>30835</v>
       </c>
       <c r="D110" s="10">
-        <f t="shared" si="5"/>
-        <v>1687393</v>
+        <f>B110-C110</f>
+        <v>23582</v>
       </c>
       <c r="E110" s="11">
-        <f t="shared" si="6"/>
-        <v>4.5653460819406453</v>
+        <f>IF(C110=0,"NEW",D110/C110)</f>
+        <v>0.76478028214691096</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>106</v>
+        <v>17</v>
       </c>
       <c r="B111" s="1">
-        <v>11493449</v>
+        <v>52839</v>
       </c>
       <c r="C111" s="1">
-        <v>21069045</v>
+        <v>47349</v>
       </c>
       <c r="D111" s="10">
-        <f t="shared" si="5"/>
-        <v>-9575596</v>
+        <f>B111-C111</f>
+        <v>5490</v>
       </c>
       <c r="E111" s="11">
-        <f t="shared" si="6"/>
-        <v>-0.45448647530061281</v>
+        <f>IF(C111=0,"NEW",D111/C111)</f>
+        <v>0.11594753849078122</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>107</v>
+        <v>30</v>
       </c>
       <c r="B112" s="1">
-        <v>362631</v>
+        <v>48873</v>
       </c>
       <c r="C112" s="1">
-        <v>1915198</v>
+        <v>17070</v>
       </c>
       <c r="D112" s="10">
-        <f t="shared" si="5"/>
-        <v>-1552567</v>
+        <f>B112-C112</f>
+        <v>31803</v>
       </c>
       <c r="E112" s="11">
-        <f t="shared" si="6"/>
-        <v>-0.8106561305932859</v>
+        <f>IF(C112=0,"NEW",D112/C112)</f>
+        <v>1.8630931458699473</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>108</v>
+        <v>25</v>
       </c>
       <c r="B113" s="1">
-        <v>526282</v>
+        <v>36527</v>
       </c>
       <c r="C113" s="1">
-        <v>395395</v>
+        <v>0</v>
       </c>
       <c r="D113" s="10">
-        <f t="shared" si="5"/>
-        <v>130887</v>
-      </c>
-      <c r="E113" s="11">
-        <f t="shared" si="6"/>
-        <v>0.33102846520568041</v>
+        <f>B113-C113</f>
+        <v>36527</v>
+      </c>
+      <c r="E113" s="11" t="str">
+        <f>IF(C113=0,"NEW",D113/C113)</f>
+        <v>NEW</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>109</v>
+        <v>88</v>
       </c>
       <c r="B114" s="1">
-        <v>99385</v>
+        <v>23793</v>
       </c>
       <c r="C114" s="1">
         <v>0</v>
       </c>
       <c r="D114" s="10">
-        <f t="shared" si="5"/>
-        <v>99385</v>
+        <f>B114-C114</f>
+        <v>23793</v>
       </c>
       <c r="E114" s="11" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(C114=0,"NEW",D114/C114)</f>
         <v>NEW</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>110</v>
+        <v>50</v>
       </c>
       <c r="B115" s="1">
-        <v>5135706</v>
+        <v>22973</v>
       </c>
       <c r="C115" s="1">
-        <v>7482088</v>
+        <v>11776</v>
       </c>
       <c r="D115" s="10">
-        <f t="shared" si="5"/>
-        <v>-2346382</v>
+        <f>B115-C115</f>
+        <v>11197</v>
       </c>
       <c r="E115" s="11">
-        <f t="shared" si="6"/>
-        <v>-0.31359989350566314</v>
+        <f>IF(C115=0,"NEW",D115/C115)</f>
+        <v>0.95083220108695654</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>111</v>
+        <v>66</v>
       </c>
       <c r="B116" s="1">
-        <v>196000</v>
+        <v>18300</v>
       </c>
       <c r="C116" s="1">
-        <v>91056</v>
+        <v>29625</v>
       </c>
       <c r="D116" s="10">
-        <f t="shared" si="5"/>
-        <v>104944</v>
+        <f>B116-C116</f>
+        <v>-11325</v>
       </c>
       <c r="E116" s="11">
-        <f t="shared" si="6"/>
-        <v>1.1525215252152521</v>
+        <f>IF(C116=0,"NEW",D116/C116)</f>
+        <v>-0.38227848101265821</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>112</v>
+        <v>45</v>
       </c>
       <c r="B117" s="1">
-        <v>8526853</v>
+        <v>14655</v>
       </c>
       <c r="C117" s="1">
-        <v>10739227</v>
+        <v>64583</v>
       </c>
       <c r="D117" s="10">
-        <f t="shared" si="5"/>
-        <v>-2212374</v>
+        <f>B117-C117</f>
+        <v>-49928</v>
       </c>
       <c r="E117" s="11">
-        <f t="shared" si="6"/>
-        <v>-0.20600868200290393</v>
+        <f>IF(C117=0,"NEW",D117/C117)</f>
+        <v>-0.77308269978167632</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>113</v>
+        <v>53</v>
       </c>
       <c r="B118" s="1">
-        <v>698561</v>
+        <v>12608</v>
       </c>
       <c r="C118" s="1">
-        <v>1130404</v>
+        <v>6780</v>
       </c>
       <c r="D118" s="10">
-        <f t="shared" si="5"/>
-        <v>-431843</v>
+        <f>B118-C118</f>
+        <v>5828</v>
       </c>
       <c r="E118" s="11">
-        <f t="shared" si="6"/>
-        <v>-0.38202536438299933</v>
+        <f>IF(C118=0,"NEW",D118/C118)</f>
+        <v>0.85958702064896753</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>114</v>
+        <v>128</v>
       </c>
       <c r="B119" s="1">
-        <v>0</v>
+        <v>10605</v>
       </c>
       <c r="C119" s="1">
-        <v>4779</v>
+        <v>8760</v>
       </c>
       <c r="D119" s="10">
-        <f t="shared" si="5"/>
-        <v>-4779</v>
+        <f>B119-C119</f>
+        <v>1845</v>
       </c>
       <c r="E119" s="11">
-        <f t="shared" si="6"/>
-        <v>-1</v>
+        <f>IF(C119=0,"NEW",D119/C119)</f>
+        <v>0.21061643835616439</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>115</v>
+        <v>71</v>
       </c>
       <c r="B120" s="1">
-        <v>15921847</v>
+        <v>9098</v>
       </c>
       <c r="C120" s="1">
-        <v>25699820</v>
+        <v>0</v>
       </c>
       <c r="D120" s="10">
-        <f t="shared" si="5"/>
-        <v>-9777973</v>
-      </c>
-      <c r="E120" s="11">
-        <f t="shared" si="6"/>
-        <v>-0.38046854024658538</v>
+        <f>B120-C120</f>
+        <v>9098</v>
+      </c>
+      <c r="E120" s="11" t="str">
+        <f>IF(C120=0,"NEW",D120/C120)</f>
+        <v>NEW</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>116</v>
+        <v>79</v>
       </c>
       <c r="B121" s="1">
-        <v>3550</v>
+        <v>8235</v>
       </c>
       <c r="C121" s="1">
-        <v>68800</v>
+        <v>12046</v>
       </c>
       <c r="D121" s="10">
-        <f t="shared" si="5"/>
-        <v>-65250</v>
+        <f>B121-C121</f>
+        <v>-3811</v>
       </c>
       <c r="E121" s="11">
-        <f t="shared" si="6"/>
-        <v>-0.94840116279069764</v>
+        <f>IF(C121=0,"NEW",D121/C121)</f>
+        <v>-0.3163705794454591</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>117</v>
+        <v>134</v>
       </c>
       <c r="B122" s="1">
-        <v>1187314</v>
+        <v>7993</v>
       </c>
       <c r="C122" s="1">
-        <v>2419716</v>
+        <v>0</v>
       </c>
       <c r="D122" s="10">
-        <f t="shared" si="5"/>
-        <v>-1232402</v>
-      </c>
-      <c r="E122" s="11">
-        <f t="shared" si="6"/>
-        <v>-0.50931679585538137</v>
+        <f>B122-C122</f>
+        <v>7993</v>
+      </c>
+      <c r="E122" s="11" t="str">
+        <f>IF(C122=0,"NEW",D122/C122)</f>
+        <v>NEW</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>118</v>
+        <v>85</v>
       </c>
       <c r="B123" s="1">
-        <v>1984453</v>
+        <v>7800</v>
       </c>
       <c r="C123" s="1">
-        <v>2408698</v>
+        <v>19210</v>
       </c>
       <c r="D123" s="10">
-        <f t="shared" si="5"/>
-        <v>-424245</v>
+        <f>B123-C123</f>
+        <v>-11410</v>
       </c>
       <c r="E123" s="11">
-        <f t="shared" si="6"/>
-        <v>-0.1761304239883954</v>
+        <f>IF(C123=0,"NEW",D123/C123)</f>
+        <v>-0.59396147839666835</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>119</v>
+        <v>98</v>
       </c>
       <c r="B124" s="1">
-        <v>68291120</v>
+        <v>7740</v>
       </c>
       <c r="C124" s="1">
-        <v>75674760</v>
+        <v>0</v>
       </c>
       <c r="D124" s="10">
-        <f t="shared" si="5"/>
-        <v>-7383640</v>
-      </c>
-      <c r="E124" s="11">
-        <f t="shared" si="6"/>
-        <v>-9.7570709177009607E-2</v>
+        <f>B124-C124</f>
+        <v>7740</v>
+      </c>
+      <c r="E124" s="11" t="str">
+        <f>IF(C124=0,"NEW",D124/C124)</f>
+        <v>NEW</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="B125" s="1">
-        <v>576160</v>
+        <v>5935</v>
       </c>
       <c r="C125" s="1">
-        <v>395859</v>
+        <v>12231</v>
       </c>
       <c r="D125" s="10">
-        <f t="shared" si="5"/>
-        <v>180301</v>
+        <f>B125-C125</f>
+        <v>-6296</v>
       </c>
       <c r="E125" s="11">
-        <f t="shared" si="6"/>
-        <v>0.4554677296714234</v>
+        <f>IF(C125=0,"NEW",D125/C125)</f>
+        <v>-0.51475758319025422</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
       <c r="B126" s="1">
-        <v>0</v>
+        <v>5746</v>
       </c>
       <c r="C126" s="1">
-        <v>22641</v>
+        <v>132515</v>
       </c>
       <c r="D126" s="10">
-        <f t="shared" si="5"/>
-        <v>-22641</v>
+        <f>B126-C126</f>
+        <v>-126769</v>
       </c>
       <c r="E126" s="11">
-        <f t="shared" si="6"/>
-        <v>-1</v>
+        <f>IF(C126=0,"NEW",D126/C126)</f>
+        <v>-0.95663887107119949</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="B127" s="1">
-        <v>88919</v>
+        <v>3550</v>
       </c>
       <c r="C127" s="1">
-        <v>81554</v>
+        <v>68800</v>
       </c>
       <c r="D127" s="10">
-        <f t="shared" si="5"/>
-        <v>7365</v>
+        <f>B127-C127</f>
+        <v>-65250</v>
       </c>
       <c r="E127" s="11">
-        <f t="shared" si="6"/>
-        <v>9.030826201044706E-2</v>
+        <f>IF(C127=0,"NEW",D127/C127)</f>
+        <v>-0.94840116279069764</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>123</v>
+        <v>99</v>
       </c>
       <c r="B128" s="1">
-        <v>352259</v>
+        <v>0</v>
       </c>
       <c r="C128" s="1">
-        <v>479898</v>
+        <v>1075001</v>
       </c>
       <c r="D128" s="10">
-        <f t="shared" si="5"/>
-        <v>-127639</v>
+        <f>B128-C128</f>
+        <v>-1075001</v>
       </c>
       <c r="E128" s="11">
-        <f t="shared" si="6"/>
-        <v>-0.26597110219254927</v>
+        <f>IF(C128=0,"NEW",D128/C128)</f>
+        <v>-1</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>124</v>
+        <v>15</v>
       </c>
       <c r="B129" s="1">
-        <v>2012417</v>
+        <v>0</v>
       </c>
       <c r="C129" s="1">
-        <v>2473638</v>
+        <v>153007</v>
       </c>
       <c r="D129" s="10">
-        <f t="shared" si="5"/>
-        <v>-461221</v>
+        <f>B129-C129</f>
+        <v>-153007</v>
       </c>
       <c r="E129" s="11">
-        <f t="shared" si="6"/>
-        <v>-0.18645452568241594</v>
+        <f>IF(C129=0,"NEW",D129/C129)</f>
+        <v>-1</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>125</v>
+        <v>31</v>
       </c>
       <c r="B130" s="1">
-        <v>6880238</v>
+        <v>0</v>
       </c>
       <c r="C130" s="1">
-        <v>10889924</v>
+        <v>143790</v>
       </c>
       <c r="D130" s="10">
-        <f t="shared" si="5"/>
-        <v>-4009686</v>
+        <f>B130-C130</f>
+        <v>-143790</v>
       </c>
       <c r="E130" s="11">
-        <f t="shared" si="6"/>
-        <v>-0.3682014677053761</v>
+        <f>IF(C130=0,"NEW",D130/C130)</f>
+        <v>-1</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
       <c r="B131" s="1">
-        <v>914003</v>
+        <v>0</v>
       </c>
       <c r="C131" s="1">
-        <v>1290126</v>
+        <v>133885</v>
       </c>
       <c r="D131" s="10">
-        <f t="shared" si="5"/>
-        <v>-376123</v>
+        <f>B131-C131</f>
+        <v>-133885</v>
       </c>
       <c r="E131" s="11">
-        <f t="shared" si="6"/>
-        <v>-0.29153974107955349</v>
+        <f>IF(C131=0,"NEW",D131/C131)</f>
+        <v>-1</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>127</v>
+        <v>16</v>
       </c>
       <c r="B132" s="1">
-        <v>2089751</v>
+        <v>0</v>
       </c>
       <c r="C132" s="1">
-        <v>2693769</v>
+        <v>115461</v>
       </c>
       <c r="D132" s="10">
-        <f t="shared" si="5"/>
-        <v>-604018</v>
+        <f>B132-C132</f>
+        <v>-115461</v>
       </c>
       <c r="E132" s="11">
-        <f t="shared" si="6"/>
-        <v>-0.22422783839297283</v>
+        <f>IF(C132=0,"NEW",D132/C132)</f>
+        <v>-1</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>128</v>
+        <v>19</v>
       </c>
       <c r="B133" s="1">
-        <v>10605</v>
+        <v>0</v>
       </c>
       <c r="C133" s="1">
-        <v>8760</v>
+        <v>41640</v>
       </c>
       <c r="D133" s="10">
-        <f t="shared" si="5"/>
-        <v>1845</v>
+        <f>B133-C133</f>
+        <v>-41640</v>
       </c>
       <c r="E133" s="11">
-        <f t="shared" si="6"/>
-        <v>0.21061643835616439</v>
+        <f>IF(C133=0,"NEW",D133/C133)</f>
+        <v>-1</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>129</v>
+        <v>95</v>
       </c>
       <c r="B134" s="1">
         <v>0</v>
       </c>
       <c r="C134" s="1">
-        <v>7800</v>
+        <v>36935</v>
       </c>
       <c r="D134" s="10">
-        <f t="shared" si="5"/>
-        <v>-7800</v>
+        <f>B134-C134</f>
+        <v>-36935</v>
       </c>
       <c r="E134" s="11">
-        <f t="shared" si="6"/>
+        <f>IF(C134=0,"NEW",D134/C134)</f>
         <v>-1</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>130</v>
+        <v>97</v>
       </c>
       <c r="B135" s="1">
-        <v>5935</v>
+        <v>0</v>
       </c>
       <c r="C135" s="1">
-        <v>12231</v>
+        <v>35986</v>
       </c>
       <c r="D135" s="10">
-        <f t="shared" si="5"/>
-        <v>-6296</v>
+        <f>B135-C135</f>
+        <v>-35986</v>
       </c>
       <c r="E135" s="11">
-        <f t="shared" si="6"/>
-        <v>-0.51475758319025422</v>
+        <f>IF(C135=0,"NEW",D135/C135)</f>
+        <v>-1</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>131</v>
+        <v>41</v>
       </c>
       <c r="B136" s="1">
-        <v>12644240</v>
+        <v>0</v>
       </c>
       <c r="C136" s="1">
-        <v>15462991</v>
+        <v>34450</v>
       </c>
       <c r="D136" s="10">
-        <f t="shared" si="5"/>
-        <v>-2818751</v>
+        <f>B136-C136</f>
+        <v>-34450</v>
       </c>
       <c r="E136" s="11">
-        <f t="shared" si="6"/>
-        <v>-0.18229015330863221</v>
+        <f>IF(C136=0,"NEW",D136/C136)</f>
+        <v>-1</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>132</v>
+        <v>101</v>
       </c>
       <c r="B137" s="1">
-        <v>9705218</v>
+        <v>0</v>
       </c>
       <c r="C137" s="1">
-        <v>12788525</v>
+        <v>28041</v>
       </c>
       <c r="D137" s="10">
-        <f t="shared" si="5"/>
-        <v>-3083307</v>
+        <f>B137-C137</f>
+        <v>-28041</v>
       </c>
       <c r="E137" s="11">
-        <f t="shared" si="6"/>
-        <v>-0.24109950131074537</v>
+        <f>IF(C137=0,"NEW",D137/C137)</f>
+        <v>-1</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="B138" s="1">
-        <v>113844796</v>
+        <v>0</v>
       </c>
       <c r="C138" s="1">
-        <v>157863431</v>
+        <v>22641</v>
       </c>
       <c r="D138" s="10">
-        <f t="shared" si="5"/>
-        <v>-44018635</v>
+        <f>B138-C138</f>
+        <v>-22641</v>
       </c>
       <c r="E138" s="11">
-        <f t="shared" si="6"/>
-        <v>-0.27883997402793048</v>
+        <f>IF(C138=0,"NEW",D138/C138)</f>
+        <v>-1</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>134</v>
+        <v>61</v>
       </c>
       <c r="B139" s="1">
-        <v>7993</v>
+        <v>0</v>
       </c>
       <c r="C139" s="1">
-        <v>0</v>
+        <v>9251</v>
       </c>
       <c r="D139" s="10">
-        <f t="shared" si="5"/>
-        <v>7993</v>
-      </c>
-      <c r="E139" s="11" t="str">
-        <f t="shared" si="6"/>
-        <v>NEW</v>
+        <f>B139-C139</f>
+        <v>-9251</v>
+      </c>
+      <c r="E139" s="11">
+        <f>IF(C139=0,"NEW",D139/C139)</f>
+        <v>-1</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B140" s="1">
-        <v>68387</v>
+        <v>0</v>
       </c>
       <c r="C140" s="1">
-        <v>352823</v>
+        <v>7800</v>
       </c>
       <c r="D140" s="10">
-        <f t="shared" si="5"/>
-        <v>-284436</v>
+        <f>B140-C140</f>
+        <v>-7800</v>
       </c>
       <c r="E140" s="11">
-        <f t="shared" si="6"/>
-        <v>-0.80617193323564507</v>
+        <f>IF(C140=0,"NEW",D140/C140)</f>
+        <v>-1</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>136</v>
+        <v>35</v>
       </c>
       <c r="B141" s="1">
-        <v>3843945</v>
+        <v>0</v>
       </c>
       <c r="C141" s="1">
-        <v>3307725</v>
+        <v>7737</v>
       </c>
       <c r="D141" s="10">
-        <f t="shared" si="5"/>
-        <v>536220</v>
+        <f>B141-C141</f>
+        <v>-7737</v>
       </c>
       <c r="E141" s="11">
-        <f t="shared" si="6"/>
-        <v>0.16211142099176926</v>
+        <f>IF(C141=0,"NEW",D141/C141)</f>
+        <v>-1</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>137</v>
+        <v>114</v>
       </c>
       <c r="B142" s="1">
         <v>0</v>
       </c>
       <c r="C142" s="1">
-        <v>133885</v>
+        <v>4779</v>
       </c>
       <c r="D142" s="10">
-        <f t="shared" si="5"/>
-        <v>-133885</v>
+        <f>B142-C142</f>
+        <v>-4779</v>
       </c>
       <c r="E142" s="11">
-        <f t="shared" si="6"/>
+        <f>IF(C142=0,"NEW",D142/C142)</f>
         <v>-1</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>138</v>
+        <v>64</v>
       </c>
       <c r="B143" s="1">
-        <v>450663</v>
+        <v>0</v>
       </c>
       <c r="C143" s="1">
-        <v>449503</v>
+        <v>3037</v>
       </c>
       <c r="D143" s="10">
-        <f t="shared" si="5"/>
-        <v>1160</v>
+        <f>B143-C143</f>
+        <v>-3037</v>
       </c>
       <c r="E143" s="11">
-        <f t="shared" si="6"/>
-        <v>2.5806279379670437E-3</v>
+        <f>IF(C143=0,"NEW",D143/C143)</f>
+        <v>-1</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.3">
@@ -10971,21 +11606,28 @@
         <v>1021250075</v>
       </c>
       <c r="D144" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="D85:D144" si="2">B144-C144</f>
         <v>-298494991</v>
       </c>
       <c r="E144" s="11">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="E85:E144" si="3">IF(C144=0,"NEW",D144/C144)</f>
         <v>-0.29228393545038417</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="5">
+    <mergeCell ref="G61:K61"/>
     <mergeCell ref="A1:E1"/>
+    <mergeCell ref="H35:I35"/>
+    <mergeCell ref="H23:K23"/>
+    <mergeCell ref="G47:K47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -11352,7 +11994,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+    <sheetView topLeftCell="A61" workbookViewId="0">
       <selection activeCell="Q42" sqref="Q42"/>
     </sheetView>
   </sheetViews>

</xml_diff>